<commit_message>
Update Ket qua va code
- Update ham EigenClassifier_new : thu cac cach tinh eigs va kich thuoc
luu tru Q, P
- Cap nhat ket qua tren Caltech 256 o Sheet Caltech256_new ( 3 phương
pháp)
</commit_message>
<xml_diff>
--- a/KetquatrenCaltech256 (Autosaved).xlsx
+++ b/KetquatrenCaltech256 (Autosaved).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="330" windowWidth="15120" windowHeight="7185"/>
+    <workbookView xWindow="240" yWindow="330" windowWidth="15120" windowHeight="7185" firstSheet="2" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Flat" sheetId="1" r:id="rId1"/>
@@ -15,13 +15,15 @@
     <sheet name="Sheet1" sheetId="14" r:id="rId6"/>
     <sheet name="Sheet2" sheetId="15" r:id="rId7"/>
     <sheet name="Sheet3" sheetId="16" r:id="rId8"/>
+    <sheet name="ILSVRC_new" sheetId="19" r:id="rId9"/>
+    <sheet name="Caltech256_new" sheetId="17" r:id="rId10"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="269">
   <si>
     <t>Tỉ lệ train/val/test: 50%-25%-25%</t>
   </si>
@@ -565,6 +567,270 @@
   </si>
   <si>
     <t xml:space="preserve">    0.1141    0.1432    0.2151    0.2710    0.3418    0.3746    0.3913    0.4061</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.0833    0.1016    0.1467    0.1645    0.1829    0.1902    0.1948    0.1976    0.2004    0.2026    0.2042    0.2056    0.2065</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.1941    0.2332    0.2969    0.3564    0.4043    0.4256    0.4322    0.4391</t>
+  </si>
+  <si>
+    <t>32-new</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.0033    0.0041    0.0037    0.0035    0.0053    0.0049    0.0041    0.0053</t>
+  </si>
+  <si>
+    <t>32-new*1000</t>
+  </si>
+  <si>
+    <t>Thực hiện với tỉ lệ train/test/val = 40/20/20 ảnh ( lý do: tối thiểu 80 ảnh/class)</t>
+  </si>
+  <si>
+    <t>App1 ( không scale giá trị của ma trận U khi train regresser)</t>
+  </si>
+  <si>
+    <t>App1 ( scale giá trị của ma trận U=U*1000 khi train regresser)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.1877    0.2264    0.2865    0.3463    0.3937    0.4092    0.4156    0.4227</t>
+  </si>
+  <si>
+    <t>App1 ( scale giá trị của ma trận U=U*256 khi train regresser)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.0039    0.0039    0.0039    0.0039    0.0039    0.0039    0.0039    0.0039</t>
+  </si>
+  <si>
+    <t>Flat</t>
+  </si>
+  <si>
+    <t>App1 ( scale giá trị của ma trận U=U*100 khi train regresser)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.1857    0.2236    0.2865    0.3441    0.3912    0.4068    0.4143    0.4209</t>
+  </si>
+  <si>
+    <t>App1 ( scale giá trị của ma trận U=U*10.000 khi train regresser)</t>
+  </si>
+  <si>
+    <t>App1 ( scale giá trị của ma trận U=U*1.000 khi train regresser)</t>
+  </si>
+  <si>
+    <t>0.1896    0.2264    0.2885    0.3486    0.3937    0.4109    0.4172    0.4246</t>
+  </si>
+  <si>
+    <t>Thực hiện với tỉ lệ train/test/val =100/150/30 ảnh</t>
+  </si>
+  <si>
+    <t>0.1896    0.2301    0.2961    0.3516    0.4006    0.4246    0.4313    0.4361</t>
+  </si>
+  <si>
+    <t>0.1896    0.2301    0.2961    0.3516    0.4006    0.4246    0.4344    0.4361</t>
+  </si>
+  <si>
+    <t>0.1081    0.1387    0.2032    0.2555    0.3199    0.3499    0.3634    0.3757</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MainClassify(1,1,256,1,0,33,0,4); </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MainClassify(1,1,256,1,0,33,0,2); </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MainClassify(1,1,256,1,0,33,1,2); </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MainClassify(1,1,256,1,0,33,1,4); </t>
+  </si>
+  <si>
+    <t>MainClassify(1,1,256,1,0,33,0,1);</t>
+  </si>
+  <si>
+    <t>MainClassify(1,1,256,1,0,33,0,3);</t>
+  </si>
+  <si>
+    <t>MainClassify(1,1,256,1,0,33,1,1);</t>
+  </si>
+  <si>
+    <t>MainClassify(1,1,256,1,0,33,1,3);</t>
+  </si>
+  <si>
+    <t>Kernel</t>
+  </si>
+  <si>
+    <t>0.1081    0.1387    0.2032    0.2555    0.3200    0.3499    0.3636    0.3757</t>
+  </si>
+  <si>
+    <t>0.1896    0.2301    0.2961    0.3516    0.4025    0.4246    0.4342    0.4361</t>
+  </si>
+  <si>
+    <t>0.1081    0.1387    0.2032    0.2555    0.3208    0.3499    0.3636    0.3757</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.1084    0.1387    0.2032    0.2555    0.3199    0.3499    0.3639    0.3757</t>
+  </si>
+  <si>
+    <t>0.1975    0.2301    0.2961    0.3516    0.4006    0.4246    0.4326    0.4361</t>
+  </si>
+  <si>
+    <t>[VVk,DDk] = eigs(P,Q,L);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[VVk,DDk] = eigs(Pk,Qk,L); </t>
+  </si>
+  <si>
+    <t>[VVk,DDk] = eigs(Q_iP,L);</t>
+  </si>
+  <si>
+    <t>[VVk,DDk] = eigs(Qk_iPk,L);</t>
+  </si>
+  <si>
+    <t>0.1082    0.1390    0.2035    0.2558    0.3200    0.3499    0.3639    0.3757</t>
+  </si>
+  <si>
+    <t>0.0067    0.0067    0.0064    0.0063    0.0065    0.0056    0.0066    0.0052</t>
+  </si>
+  <si>
+    <t>0.1898    0.2303    0.2961    0.3514    0.4006    0.4246    0.4324    0.4359</t>
+  </si>
+  <si>
+    <t>0.1082    0.1390    0.2035    0.2558    0.3200    0.3499    0.3642    0.3757</t>
+  </si>
+  <si>
+    <t>0.0049    0.0049    0.0039    0.0055    0.0041    0.0043    0.0043    0.0041</t>
+  </si>
+  <si>
+    <t>0.1898    0.2303    0.2961    0.3514    0.4006    0.4246    0.4330    0.4361</t>
+  </si>
+  <si>
+    <t>0.0039    0.0039    0.0039    0.0039    0.0039    0.0039    0.0039    0.0039</t>
+  </si>
+  <si>
+    <t>0.0065    0.0065    0.0065    0.0065    0.0065    0.0065    0.0065    0.0065</t>
+  </si>
+  <si>
+    <t>MainClassify(1,1,256,1,0,32,0,1);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MainClassify(1,1,256,1,0,32,0,2); </t>
+  </si>
+  <si>
+    <t>MainClassify(1,1,256,1,0,32,0,3);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MainClassify(1,1,256,1,0,32,0,4); </t>
+  </si>
+  <si>
+    <t>MainClassify(1,1,256,1,0,32,1,1);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MainClassify(1,1,256,1,0,32,1,2); </t>
+  </si>
+  <si>
+    <t>MainClassify(1,1,256,1,0,32,1,3);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MainClassify(1,1,256,1,0,32,1,4); </t>
+  </si>
+  <si>
+    <t>SVR</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.0035    0.0031    0.0020    0.0037    0.0037    0.0031    0.0037    0.0051</t>
+  </si>
+  <si>
+    <t>0.0057    0.0055    0.0055    0.0056    0.0054    0.0055    0.0055    0.0057</t>
+  </si>
+  <si>
+    <t>0.0840    0.1018    0.1457    0.1634    0.1831    0.1905    0.1954    0.1986    0.2014    0.2038    0.2057    0.2074    0.2085</t>
+  </si>
+  <si>
+    <t>App1 ( scale giá trị của ma trận U=U*3000 khi train regresser)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      24          30           64             100            200         300         400         500          600           700         800         900        1000</t>
+  </si>
+  <si>
+    <t>0.1900    0.2264    0.2883    0.3482    0.3937    0.4102    0.4168    0.4244</t>
+  </si>
+  <si>
+    <t>Calxx(1-1000), SVR1(800-1000), SVR2(600-800),SVR3(400-600), SVR4(300-400)</t>
+  </si>
+  <si>
+    <t>MainClassify(1,1,256,1,0,32,0,2);</t>
+  </si>
+  <si>
+    <t>0.1941    0.2332    0.2969    0.3564    0.4043    0.4256    0.4322    0.4391</t>
+  </si>
+  <si>
+    <t>0.0849    0.1132    0.1760    0.2354    0.3052    0.3349    0.3521    0.3645</t>
+  </si>
+  <si>
+    <t>MainClassify(1,1,256,1,0,32,0,4);</t>
+  </si>
+  <si>
+    <t>MainClassify(1,1,256,1,0,32,1,2);</t>
+  </si>
+  <si>
+    <t>MainClassify(1,1,256,1,0,32,1,4);</t>
+  </si>
+  <si>
+    <t>0.0031    0.0049    0.0053    0.0037    0.0035    0.0035    0.0033    0.0045</t>
+  </si>
+  <si>
+    <t>0.0054    0.0056    0.0057    0.0058    0.0059    0.0056    0.0057    0.0058</t>
+  </si>
+  <si>
+    <t>Accucary</t>
+  </si>
+  <si>
+    <t>0.1916    0.2322    0.2975    0.3561    0.4041    0.4250    0.4314    0.4391</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.0855    0.1103    0.1718    0.2251    0.2907    0.3228    0.3393    0.3511</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.0039    0.0037    0.0031    0.0033    0.0045    0.0045    0.0041    0.0045</t>
+  </si>
+  <si>
+    <t>0.0055    0.0056    0.0055    0.0054    0.0050    0.0052    0.0053    0.0055</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.1916    0.2322    0.2975    0.3561    0.4041    0.4250    0.4314    0.4391</t>
+  </si>
+  <si>
+    <t>0.0855    0.1103    0.1718    0.2251    0.2907    0.3228    0.3393    0.3511</t>
+  </si>
+  <si>
+    <t>0.0020    0.0049    0.0043    0.0043    0.0031    0.0043    0.0041    0.0033</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.0055    0.0054    0.0055    0.0055    0.0055    0.0055    0.0055    0.0056</t>
+  </si>
+  <si>
+    <t>Kết luận</t>
+  </si>
+  <si>
+    <t>eigs(A,B) tuong đương eigs(B\A)</t>
+  </si>
+  <si>
+    <t>App1(SVR) &lt; App2(joint) ~ App(kernel)</t>
+  </si>
+  <si>
+    <t>Cần xét thêm</t>
+  </si>
+  <si>
+    <t>Tại sao  App2(joint) ~ App(kernel)</t>
+  </si>
+  <si>
+    <t>Dùng hai ma tran P,Q cho ket qua thap --&gt; P  + k và Q + k vào đường chéo chính (k=0.01)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">giá trị k có ảnh hưởng gì không </t>
+  </si>
+  <si>
+    <t>feature vectors có xét 1 ( xét bk)  cho kết quả thấp hơn không xét bk  ?</t>
   </si>
 </sst>
 </file>
@@ -853,7 +1119,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="181">
+  <cellXfs count="197">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1174,6 +1440,33 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="20" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1213,6 +1506,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1850,11 +2150,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="107166336"/>
-        <c:axId val="107180416"/>
+        <c:axId val="167710080"/>
+        <c:axId val="167724160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="107166336"/>
+        <c:axId val="167710080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1864,7 +2164,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107180416"/>
+        <c:crossAx val="167724160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1872,7 +2172,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107180416"/>
+        <c:axId val="167724160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1883,7 +2183,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107166336"/>
+        <c:crossAx val="167710080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2441,11 +2741,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="107552768"/>
-        <c:axId val="107554304"/>
+        <c:axId val="167756544"/>
+        <c:axId val="167758080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="107552768"/>
+        <c:axId val="167756544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2455,7 +2755,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107554304"/>
+        <c:crossAx val="167758080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2463,7 +2763,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107554304"/>
+        <c:axId val="167758080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2474,7 +2774,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107552768"/>
+        <c:crossAx val="167756544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3035,11 +3335,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="107586688"/>
-        <c:axId val="107588224"/>
+        <c:axId val="167532416"/>
+        <c:axId val="167533952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="107586688"/>
+        <c:axId val="167532416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3049,7 +3349,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107588224"/>
+        <c:crossAx val="167533952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3057,7 +3357,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107588224"/>
+        <c:axId val="167533952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3068,7 +3368,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107586688"/>
+        <c:crossAx val="167532416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3593,11 +3893,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="107366656"/>
-        <c:axId val="107372544"/>
+        <c:axId val="167578624"/>
+        <c:axId val="167580416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="107366656"/>
+        <c:axId val="167578624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3607,7 +3907,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107372544"/>
+        <c:crossAx val="167580416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3615,7 +3915,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107372544"/>
+        <c:axId val="167580416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3626,7 +3926,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107366656"/>
+        <c:crossAx val="167578624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3662,7 +3962,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3793,11 +4092,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="107401216"/>
-        <c:axId val="107402752"/>
+        <c:axId val="167602048"/>
+        <c:axId val="167603584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="107401216"/>
+        <c:axId val="167602048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3807,7 +4106,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107402752"/>
+        <c:crossAx val="167603584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3815,7 +4114,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107402752"/>
+        <c:axId val="167603584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3823,14 +4122,13 @@
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107401216"/>
+        <c:crossAx val="167602048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3878,7 +4176,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>eigenclass!$AC$11</c:f>
+              <c:f>eigenclass!$AC$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3892,7 +4190,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>eigenclass!$AD$10:$AK$10</c:f>
+              <c:f>eigenclass!$AD$11:$AK$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3925,7 +4223,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>eigenclass!$AD$11:$AK$11</c:f>
+              <c:f>eigenclass!$AD$12:$AK$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3963,7 +4261,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>eigenclass!$AC$12</c:f>
+              <c:f>eigenclass!$AC$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3977,7 +4275,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>eigenclass!$AD$10:$AK$10</c:f>
+              <c:f>eigenclass!$AD$11:$AK$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4010,7 +4308,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>eigenclass!$AD$12:$AK$12</c:f>
+              <c:f>eigenclass!$AD$13:$AK$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4048,7 +4346,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>eigenclass!$AC$17</c:f>
+              <c:f>eigenclass!$AC$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4071,7 +4369,7 @@
           </c:dPt>
           <c:cat>
             <c:numRef>
-              <c:f>eigenclass!$AD$10:$AK$10</c:f>
+              <c:f>eigenclass!$AD$11:$AK$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4104,7 +4402,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>eigenclass!$AD$17:$AK$17</c:f>
+              <c:f>eigenclass!$AD$18:$AK$18</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
@@ -4114,7 +4412,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>eigenclass!$AC$22</c:f>
+              <c:f>eigenclass!$AC$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4128,7 +4426,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>eigenclass!$AD$10:$AK$10</c:f>
+              <c:f>eigenclass!$AD$11:$AK$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4161,7 +4459,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>eigenclass!$AD$22:$AK$22</c:f>
+              <c:f>eigenclass!$AD$23:$AK$23</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4204,11 +4502,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="99637504"/>
-        <c:axId val="99643392"/>
+        <c:axId val="174519040"/>
+        <c:axId val="174520576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="99637504"/>
+        <c:axId val="174519040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4218,7 +4516,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99643392"/>
+        <c:crossAx val="174520576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4226,7 +4524,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99643392"/>
+        <c:axId val="174520576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4237,7 +4535,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99637504"/>
+        <c:crossAx val="174519040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4287,7 +4585,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>eigenclass!$B$11</c:f>
+              <c:f>eigenclass!$B$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4301,7 +4599,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>eigenclass!$C$10:$J$10</c:f>
+              <c:f>eigenclass!$C$11:$J$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4334,7 +4632,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>eigenclass!$C$11:$J$11</c:f>
+              <c:f>eigenclass!$C$12:$J$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4372,7 +4670,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>eigenclass!$B$12</c:f>
+              <c:f>eigenclass!$B$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4386,7 +4684,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>eigenclass!$C$10:$J$10</c:f>
+              <c:f>eigenclass!$C$11:$J$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4419,7 +4717,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>eigenclass!$C$12:$J$12</c:f>
+              <c:f>eigenclass!$C$13:$J$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4457,7 +4755,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>eigenclass!$B$17</c:f>
+              <c:f>eigenclass!$B$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4471,7 +4769,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>eigenclass!$C$10:$J$10</c:f>
+              <c:f>eigenclass!$C$11:$J$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4504,7 +4802,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>eigenclass!$C$17:$J$17</c:f>
+              <c:f>eigenclass!$C$18:$J$18</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
@@ -4514,7 +4812,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>eigenclass!$B$22</c:f>
+              <c:f>eigenclass!$B$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4528,7 +4826,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>eigenclass!$C$10:$J$10</c:f>
+              <c:f>eigenclass!$C$11:$J$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4561,7 +4859,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>eigenclass!$C$22:$J$22</c:f>
+              <c:f>eigenclass!$C$23:$J$23</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4604,11 +4902,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="99669888"/>
-        <c:axId val="99671424"/>
+        <c:axId val="167783040"/>
+        <c:axId val="164630912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="99669888"/>
+        <c:axId val="167783040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4618,7 +4916,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99671424"/>
+        <c:crossAx val="164630912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4626,7 +4924,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99671424"/>
+        <c:axId val="164630912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4637,7 +4935,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99669888"/>
+        <c:crossAx val="167783040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4684,7 +4982,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>eigenclass!$M$11</c:f>
+              <c:f>eigenclass!$M$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4698,7 +4996,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>eigenclass!$N$10:$Z$10</c:f>
+              <c:f>eigenclass!$N$11:$Z$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -4746,7 +5044,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>eigenclass!$N$11:$Z$11</c:f>
+              <c:f>eigenclass!$N$12:$Z$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="13"/>
@@ -4799,7 +5097,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>eigenclass!$M$12</c:f>
+              <c:f>eigenclass!$M$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4813,7 +5111,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>eigenclass!$N$10:$Z$10</c:f>
+              <c:f>eigenclass!$N$11:$Z$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -4861,7 +5159,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>eigenclass!$N$12:$Z$12</c:f>
+              <c:f>eigenclass!$N$13:$Z$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="13"/>
@@ -4914,7 +5212,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>eigenclass!$M$17</c:f>
+              <c:f>eigenclass!$M$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4928,7 +5226,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>eigenclass!$N$10:$Z$10</c:f>
+              <c:f>eigenclass!$N$11:$Z$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -4976,7 +5274,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>eigenclass!$N$17:$Z$17</c:f>
+              <c:f>eigenclass!$N$18:$Z$18</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
@@ -4986,7 +5284,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>eigenclass!$M$22</c:f>
+              <c:f>eigenclass!$M$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5000,7 +5298,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>eigenclass!$N$10:$Z$10</c:f>
+              <c:f>eigenclass!$N$11:$Z$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -5048,7 +5346,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>eigenclass!$N$22:$Z$22</c:f>
+              <c:f>eigenclass!$N$23:$Z$23</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="13"/>
@@ -5106,11 +5404,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="99570816"/>
-        <c:axId val="99572352"/>
+        <c:axId val="167819136"/>
+        <c:axId val="167820672"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="99570816"/>
+        <c:axId val="167819136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5120,7 +5418,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99572352"/>
+        <c:crossAx val="167820672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5128,7 +5426,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99572352"/>
+        <c:axId val="167820672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5139,7 +5437,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99570816"/>
+        <c:crossAx val="167819136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5322,13 +5620,13 @@
     <xdr:from>
       <xdr:col>28</xdr:col>
       <xdr:colOff>838200</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>100011</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>36</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>104774</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5352,13 +5650,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>76202</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>447676</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>90487</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5382,13 +5680,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>1485899</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>176212</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5700,8 +5998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5916,12 +6214,346 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="59.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.44900000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="124" t="s">
+        <v>236</v>
+      </c>
+      <c r="B3" s="95" t="s">
+        <v>187</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="124"/>
+      <c r="B4" s="168" t="s">
+        <v>195</v>
+      </c>
+      <c r="C4" s="62" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="124"/>
+      <c r="B5" s="168" t="s">
+        <v>196</v>
+      </c>
+      <c r="C5" s="62" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="124"/>
+      <c r="B6" s="168" t="s">
+        <v>193</v>
+      </c>
+      <c r="C6" s="62" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="124"/>
+      <c r="B7" s="168" t="s">
+        <v>190</v>
+      </c>
+      <c r="C7" s="62" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="126"/>
+      <c r="B8" s="179"/>
+      <c r="C8" s="170" t="s">
+        <v>252</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>32</v>
+      </c>
+      <c r="B9" s="195" t="s">
+        <v>228</v>
+      </c>
+      <c r="C9" s="71" t="s">
+        <v>237</v>
+      </c>
+      <c r="D9" s="71" t="s">
+        <v>238</v>
+      </c>
+      <c r="E9" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="195" t="s">
+        <v>244</v>
+      </c>
+      <c r="C10" s="71" t="s">
+        <v>245</v>
+      </c>
+      <c r="D10" s="71" t="s">
+        <v>246</v>
+      </c>
+      <c r="E10" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="195" t="s">
+        <v>230</v>
+      </c>
+      <c r="C11" s="71" t="s">
+        <v>250</v>
+      </c>
+      <c r="D11" s="71" t="s">
+        <v>251</v>
+      </c>
+      <c r="E11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="195" t="s">
+        <v>247</v>
+      </c>
+      <c r="C12" s="71" t="s">
+        <v>182</v>
+      </c>
+      <c r="D12" s="71" t="s">
+        <v>246</v>
+      </c>
+      <c r="E12" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="194" t="s">
+        <v>232</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="194" t="s">
+        <v>248</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="194" t="s">
+        <v>234</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="194" t="s">
+        <v>249</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>210</v>
+      </c>
+      <c r="B18" s="171" t="s">
+        <v>206</v>
+      </c>
+      <c r="C18" s="172" t="s">
+        <v>212</v>
+      </c>
+      <c r="D18" s="172" t="s">
+        <v>213</v>
+      </c>
+      <c r="E18" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="172" t="s">
+        <v>203</v>
+      </c>
+      <c r="C19" s="172" t="s">
+        <v>215</v>
+      </c>
+      <c r="D19" s="172" t="s">
+        <v>214</v>
+      </c>
+      <c r="E19" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="171" t="s">
+        <v>207</v>
+      </c>
+      <c r="C20" s="172" t="s">
+        <v>199</v>
+      </c>
+      <c r="D20" s="172" t="s">
+        <v>211</v>
+      </c>
+      <c r="E20" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="172" t="s">
+        <v>202</v>
+      </c>
+      <c r="C21" s="174" t="s">
+        <v>200</v>
+      </c>
+      <c r="D21" s="172" t="s">
+        <v>201</v>
+      </c>
+      <c r="E21" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="169" t="s">
+        <v>208</v>
+      </c>
+      <c r="C22" s="73" t="s">
+        <v>226</v>
+      </c>
+      <c r="D22" s="73" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="173" t="s">
+        <v>204</v>
+      </c>
+      <c r="C23" s="73" t="s">
+        <v>222</v>
+      </c>
+      <c r="D23" s="73" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="169" t="s">
+        <v>209</v>
+      </c>
+      <c r="C24" s="73" t="s">
+        <v>224</v>
+      </c>
+      <c r="D24" s="73" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="173" t="s">
+        <v>205</v>
+      </c>
+      <c r="C25" s="173" t="s">
+        <v>225</v>
+      </c>
+      <c r="D25" s="73" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="196" t="s">
+        <v>261</v>
+      </c>
+      <c r="C28" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>264</v>
+      </c>
+      <c r="C32" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>267</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5948,49 +6580,49 @@
       </c>
     </row>
     <row r="2" spans="1:29" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="170" t="s">
+      <c r="C2" s="183" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
+      <c r="D2" s="183"/>
+      <c r="E2" s="183"/>
+      <c r="F2" s="183"/>
       <c r="G2" s="44" t="s">
         <v>15</v>
       </c>
       <c r="H2" s="66" t="s">
         <v>68</v>
       </c>
-      <c r="K2" s="170" t="s">
+      <c r="K2" s="183" t="s">
         <v>72</v>
       </c>
-      <c r="L2" s="170"/>
-      <c r="M2" s="170"/>
+      <c r="L2" s="183"/>
+      <c r="M2" s="183"/>
       <c r="N2" s="44" t="s">
         <v>15</v>
       </c>
       <c r="O2" s="66" t="s">
         <v>68</v>
       </c>
-      <c r="R2" s="170" t="s">
+      <c r="R2" s="183" t="s">
         <v>72</v>
       </c>
-      <c r="S2" s="170"/>
-      <c r="T2" s="170"/>
+      <c r="S2" s="183"/>
+      <c r="T2" s="183"/>
       <c r="U2" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="V2" s="168" t="s">
+      <c r="V2" s="181" t="s">
         <v>68</v>
       </c>
-      <c r="Y2" s="170" t="s">
+      <c r="Y2" s="183" t="s">
         <v>72</v>
       </c>
-      <c r="Z2" s="170"/>
-      <c r="AA2" s="170"/>
+      <c r="Z2" s="183"/>
+      <c r="AA2" s="183"/>
       <c r="AB2" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="AC2" s="168" t="s">
+      <c r="AC2" s="181" t="s">
         <v>68</v>
       </c>
     </row>
@@ -6030,7 +6662,7 @@
         <v>63</v>
       </c>
       <c r="U3" s="44"/>
-      <c r="V3" s="169"/>
+      <c r="V3" s="182"/>
       <c r="Y3" s="9" t="s">
         <v>84</v>
       </c>
@@ -6041,7 +6673,7 @@
         <v>86</v>
       </c>
       <c r="AB3" s="44"/>
-      <c r="AC3" s="169"/>
+      <c r="AC3" s="182"/>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -7232,44 +7864,44 @@
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
-      <c r="B6" s="172" t="s">
+      <c r="B6" s="185" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="172"/>
-      <c r="D6" s="172"/>
-      <c r="E6" s="172"/>
-      <c r="F6" s="172"/>
-      <c r="G6" s="172"/>
-      <c r="H6" s="172"/>
-      <c r="I6" s="172"/>
-      <c r="J6" s="172"/>
-      <c r="L6" s="172" t="s">
+      <c r="C6" s="185"/>
+      <c r="D6" s="185"/>
+      <c r="E6" s="185"/>
+      <c r="F6" s="185"/>
+      <c r="G6" s="185"/>
+      <c r="H6" s="185"/>
+      <c r="I6" s="185"/>
+      <c r="J6" s="185"/>
+      <c r="L6" s="185" t="s">
         <v>57</v>
       </c>
-      <c r="M6" s="172"/>
-      <c r="N6" s="172"/>
-      <c r="O6" s="172"/>
-      <c r="P6" s="172"/>
-      <c r="Q6" s="172"/>
-      <c r="R6" s="172"/>
-      <c r="S6" s="172"/>
-      <c r="T6" s="172"/>
-      <c r="U6" s="172"/>
-      <c r="V6" s="172"/>
-      <c r="W6" s="172"/>
-      <c r="X6" s="172"/>
-      <c r="Y6" s="172"/>
-      <c r="AA6" s="173" t="s">
+      <c r="M6" s="185"/>
+      <c r="N6" s="185"/>
+      <c r="O6" s="185"/>
+      <c r="P6" s="185"/>
+      <c r="Q6" s="185"/>
+      <c r="R6" s="185"/>
+      <c r="S6" s="185"/>
+      <c r="T6" s="185"/>
+      <c r="U6" s="185"/>
+      <c r="V6" s="185"/>
+      <c r="W6" s="185"/>
+      <c r="X6" s="185"/>
+      <c r="Y6" s="185"/>
+      <c r="AA6" s="186" t="s">
         <v>57</v>
       </c>
-      <c r="AB6" s="174"/>
-      <c r="AC6" s="174"/>
-      <c r="AD6" s="174"/>
-      <c r="AE6" s="174"/>
-      <c r="AF6" s="174"/>
-      <c r="AG6" s="174"/>
-      <c r="AH6" s="174"/>
-      <c r="AI6" s="175"/>
+      <c r="AB6" s="187"/>
+      <c r="AC6" s="187"/>
+      <c r="AD6" s="187"/>
+      <c r="AE6" s="187"/>
+      <c r="AF6" s="187"/>
+      <c r="AG6" s="187"/>
+      <c r="AH6" s="187"/>
+      <c r="AI6" s="188"/>
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
@@ -8088,104 +8720,104 @@
       <c r="J27" s="113"/>
     </row>
     <row r="28" spans="2:44" x14ac:dyDescent="0.25">
-      <c r="B28" s="171" t="s">
+      <c r="B28" s="184" t="s">
         <v>57</v>
       </c>
-      <c r="C28" s="171"/>
-      <c r="D28" s="171"/>
-      <c r="E28" s="171"/>
-      <c r="F28" s="171"/>
-      <c r="G28" s="171"/>
-      <c r="H28" s="171"/>
-      <c r="I28" s="171"/>
-      <c r="J28" s="171"/>
-      <c r="L28" s="171" t="s">
+      <c r="C28" s="184"/>
+      <c r="D28" s="184"/>
+      <c r="E28" s="184"/>
+      <c r="F28" s="184"/>
+      <c r="G28" s="184"/>
+      <c r="H28" s="184"/>
+      <c r="I28" s="184"/>
+      <c r="J28" s="184"/>
+      <c r="L28" s="184" t="s">
         <v>57</v>
       </c>
-      <c r="M28" s="171"/>
-      <c r="N28" s="171"/>
-      <c r="O28" s="171"/>
-      <c r="P28" s="171"/>
-      <c r="Q28" s="171"/>
-      <c r="R28" s="171"/>
-      <c r="S28" s="171"/>
-      <c r="T28" s="171"/>
+      <c r="M28" s="184"/>
+      <c r="N28" s="184"/>
+      <c r="O28" s="184"/>
+      <c r="P28" s="184"/>
+      <c r="Q28" s="184"/>
+      <c r="R28" s="184"/>
+      <c r="S28" s="184"/>
+      <c r="T28" s="184"/>
       <c r="U28" s="100"/>
       <c r="V28" s="100"/>
       <c r="W28" s="100"/>
       <c r="X28" s="100"/>
       <c r="Y28" s="100"/>
-      <c r="AA28" s="171" t="s">
+      <c r="AA28" s="184" t="s">
         <v>57</v>
       </c>
-      <c r="AB28" s="171"/>
-      <c r="AC28" s="171"/>
-      <c r="AD28" s="171"/>
-      <c r="AE28" s="171"/>
-      <c r="AF28" s="171"/>
-      <c r="AG28" s="171"/>
-      <c r="AH28" s="171"/>
-      <c r="AI28" s="171"/>
-      <c r="AK28" s="171" t="s">
+      <c r="AB28" s="184"/>
+      <c r="AC28" s="184"/>
+      <c r="AD28" s="184"/>
+      <c r="AE28" s="184"/>
+      <c r="AF28" s="184"/>
+      <c r="AG28" s="184"/>
+      <c r="AH28" s="184"/>
+      <c r="AI28" s="184"/>
+      <c r="AK28" s="184" t="s">
         <v>57</v>
       </c>
-      <c r="AL28" s="171"/>
-      <c r="AM28" s="171"/>
-      <c r="AN28" s="171"/>
-      <c r="AO28" s="171"/>
-      <c r="AP28" s="171"/>
-      <c r="AQ28" s="171"/>
-      <c r="AR28" s="171"/>
+      <c r="AL28" s="184"/>
+      <c r="AM28" s="184"/>
+      <c r="AN28" s="184"/>
+      <c r="AO28" s="184"/>
+      <c r="AP28" s="184"/>
+      <c r="AQ28" s="184"/>
+      <c r="AR28" s="184"/>
     </row>
     <row r="29" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B29" s="69"/>
-      <c r="C29" s="172" t="s">
+      <c r="C29" s="185" t="s">
         <v>7</v>
       </c>
-      <c r="D29" s="172"/>
-      <c r="E29" s="172"/>
-      <c r="F29" s="172"/>
-      <c r="G29" s="172"/>
-      <c r="H29" s="172"/>
-      <c r="I29" s="172"/>
-      <c r="J29" s="172"/>
+      <c r="D29" s="185"/>
+      <c r="E29" s="185"/>
+      <c r="F29" s="185"/>
+      <c r="G29" s="185"/>
+      <c r="H29" s="185"/>
+      <c r="I29" s="185"/>
+      <c r="J29" s="185"/>
       <c r="L29" s="69"/>
-      <c r="M29" s="172" t="s">
+      <c r="M29" s="185" t="s">
         <v>7</v>
       </c>
-      <c r="N29" s="172"/>
-      <c r="O29" s="172"/>
-      <c r="P29" s="172"/>
-      <c r="Q29" s="172"/>
-      <c r="R29" s="172"/>
-      <c r="S29" s="172"/>
-      <c r="T29" s="172"/>
+      <c r="N29" s="185"/>
+      <c r="O29" s="185"/>
+      <c r="P29" s="185"/>
+      <c r="Q29" s="185"/>
+      <c r="R29" s="185"/>
+      <c r="S29" s="185"/>
+      <c r="T29" s="185"/>
       <c r="U29" s="100"/>
       <c r="V29" s="100"/>
       <c r="W29" s="100"/>
       <c r="X29" s="100"/>
       <c r="Y29" s="100"/>
       <c r="AA29" s="69"/>
-      <c r="AB29" s="172" t="s">
+      <c r="AB29" s="185" t="s">
         <v>7</v>
       </c>
-      <c r="AC29" s="172"/>
-      <c r="AD29" s="172"/>
-      <c r="AE29" s="172"/>
-      <c r="AF29" s="172"/>
-      <c r="AG29" s="172"/>
-      <c r="AH29" s="172"/>
-      <c r="AI29" s="172"/>
+      <c r="AC29" s="185"/>
+      <c r="AD29" s="185"/>
+      <c r="AE29" s="185"/>
+      <c r="AF29" s="185"/>
+      <c r="AG29" s="185"/>
+      <c r="AH29" s="185"/>
+      <c r="AI29" s="185"/>
       <c r="AK29" s="69"/>
-      <c r="AL29" s="172" t="s">
+      <c r="AL29" s="185" t="s">
         <v>7</v>
       </c>
-      <c r="AM29" s="172"/>
-      <c r="AN29" s="172"/>
-      <c r="AO29" s="172"/>
-      <c r="AP29" s="172"/>
-      <c r="AQ29" s="172"/>
-      <c r="AR29" s="172"/>
+      <c r="AM29" s="185"/>
+      <c r="AN29" s="185"/>
+      <c r="AO29" s="185"/>
+      <c r="AP29" s="185"/>
+      <c r="AQ29" s="185"/>
+      <c r="AR29" s="185"/>
     </row>
     <row r="30" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B30" s="69"/>
@@ -9173,17 +9805,17 @@
       </c>
     </row>
     <row r="57" spans="12:25" x14ac:dyDescent="0.25">
-      <c r="L57" s="171" t="s">
+      <c r="L57" s="184" t="s">
         <v>57</v>
       </c>
-      <c r="M57" s="171"/>
-      <c r="N57" s="171"/>
-      <c r="O57" s="171"/>
-      <c r="P57" s="171"/>
-      <c r="Q57" s="171"/>
-      <c r="R57" s="171"/>
-      <c r="S57" s="171"/>
-      <c r="T57" s="171"/>
+      <c r="M57" s="184"/>
+      <c r="N57" s="184"/>
+      <c r="O57" s="184"/>
+      <c r="P57" s="184"/>
+      <c r="Q57" s="184"/>
+      <c r="R57" s="184"/>
+      <c r="S57" s="184"/>
+      <c r="T57" s="184"/>
       <c r="U57" s="100"/>
       <c r="V57" s="100"/>
       <c r="W57" s="100"/>
@@ -9192,16 +9824,16 @@
     </row>
     <row r="58" spans="12:25" x14ac:dyDescent="0.25">
       <c r="L58" s="69"/>
-      <c r="M58" s="172" t="s">
+      <c r="M58" s="185" t="s">
         <v>7</v>
       </c>
-      <c r="N58" s="172"/>
-      <c r="O58" s="172"/>
-      <c r="P58" s="172"/>
-      <c r="Q58" s="172"/>
-      <c r="R58" s="172"/>
-      <c r="S58" s="172"/>
-      <c r="T58" s="172"/>
+      <c r="N58" s="185"/>
+      <c r="O58" s="185"/>
+      <c r="P58" s="185"/>
+      <c r="Q58" s="185"/>
+      <c r="R58" s="185"/>
+      <c r="S58" s="185"/>
+      <c r="T58" s="185"/>
       <c r="U58" s="100"/>
       <c r="V58" s="100"/>
       <c r="W58" s="100"/>
@@ -9539,41 +10171,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" s="178" t="s">
+      <c r="A1" s="191" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="178" t="s">
+      <c r="B1" s="191" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="177" t="s">
+      <c r="C1" s="190" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="177"/>
-      <c r="E1" s="177"/>
-      <c r="F1" s="177"/>
-      <c r="G1" s="177"/>
-      <c r="H1" s="177"/>
-      <c r="I1" s="177"/>
-      <c r="J1" s="177"/>
-      <c r="K1" s="177"/>
-      <c r="L1" s="176" t="s">
+      <c r="D1" s="190"/>
+      <c r="E1" s="190"/>
+      <c r="F1" s="190"/>
+      <c r="G1" s="190"/>
+      <c r="H1" s="190"/>
+      <c r="I1" s="190"/>
+      <c r="J1" s="190"/>
+      <c r="K1" s="190"/>
+      <c r="L1" s="189" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="176"/>
-      <c r="N1" s="176"/>
-      <c r="O1" s="176"/>
-      <c r="P1" s="176"/>
-      <c r="Q1" s="176"/>
-      <c r="R1" s="176"/>
-      <c r="S1" s="176"/>
-      <c r="T1" s="176"/>
-      <c r="U1" s="176"/>
-      <c r="V1" s="176"/>
-      <c r="W1" s="176"/>
+      <c r="M1" s="189"/>
+      <c r="N1" s="189"/>
+      <c r="O1" s="189"/>
+      <c r="P1" s="189"/>
+      <c r="Q1" s="189"/>
+      <c r="R1" s="189"/>
+      <c r="S1" s="189"/>
+      <c r="T1" s="189"/>
+      <c r="U1" s="189"/>
+      <c r="V1" s="189"/>
+      <c r="W1" s="189"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" s="179"/>
-      <c r="B2" s="179"/>
+      <c r="A2" s="192"/>
+      <c r="B2" s="192"/>
       <c r="C2" s="30" t="s">
         <v>28</v>
       </c>
@@ -10102,10 +10734,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:BE25"/>
+  <dimension ref="B1:BE26"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:J12"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AA13" sqref="AA13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10150,451 +10782,352 @@
       </c>
     </row>
     <row r="4" spans="2:57" x14ac:dyDescent="0.25">
-      <c r="B4" s="124"/>
-      <c r="AV4" t="s">
+      <c r="B4" s="124" t="s">
+        <v>185</v>
+      </c>
+      <c r="C4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="5" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="124" t="s">
+        <v>183</v>
+      </c>
+      <c r="C5" t="s">
+        <v>182</v>
+      </c>
+      <c r="AV5" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="5" spans="2:57" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="6" spans="2:57" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>146</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>145</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AC6" t="s">
         <v>129</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AD6" t="s">
         <v>128</v>
       </c>
-      <c r="AV5" t="s">
+      <c r="AV6" t="s">
         <v>157</v>
       </c>
-      <c r="BE5">
+      <c r="BE6">
         <v>321</v>
       </c>
     </row>
-    <row r="6" spans="2:57" x14ac:dyDescent="0.25">
-      <c r="C6" s="180"/>
-      <c r="D6" s="180"/>
-      <c r="E6" s="180"/>
-      <c r="F6" s="180"/>
-      <c r="G6" s="180"/>
-      <c r="H6" s="180"/>
-      <c r="I6" s="180"/>
-      <c r="J6" s="180"/>
-      <c r="AC6" t="s">
+    <row r="7" spans="2:57" x14ac:dyDescent="0.25">
+      <c r="C7" s="193"/>
+      <c r="D7" s="193"/>
+      <c r="E7" s="193"/>
+      <c r="F7" s="193"/>
+      <c r="G7" s="193"/>
+      <c r="H7" s="193"/>
+      <c r="I7" s="193"/>
+      <c r="J7" s="193"/>
+      <c r="AC7" t="s">
         <v>148</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AD7" t="s">
         <v>147</v>
       </c>
-      <c r="AV6" t="s">
+      <c r="AV7" t="s">
         <v>158</v>
-      </c>
-    </row>
-    <row r="7" spans="2:57" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>131</v>
-      </c>
-      <c r="AC7" s="126"/>
-      <c r="AV7" t="s">
-        <v>150</v>
-      </c>
-      <c r="AY7" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="8" spans="2:57" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
+        <v>131</v>
+      </c>
+      <c r="AC8" s="126"/>
+      <c r="AV8" t="s">
+        <v>150</v>
+      </c>
+      <c r="AY8" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="2:57" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
         <v>130</v>
       </c>
-      <c r="AD8" t="s">
+      <c r="N9" t="s">
+        <v>181</v>
+      </c>
+      <c r="AD9" t="s">
         <v>132</v>
       </c>
-      <c r="AV8" t="s">
+      <c r="AV9" t="s">
         <v>152</v>
       </c>
-      <c r="AY8" t="s">
+      <c r="AY9" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="9" spans="2:57" x14ac:dyDescent="0.25">
-      <c r="M9" s="126"/>
-      <c r="AC9" s="126"/>
-    </row>
-    <row r="10" spans="2:57" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="131" t="s">
+    <row r="10" spans="2:57" x14ac:dyDescent="0.25">
+      <c r="M10" s="126"/>
+      <c r="AC10" s="126"/>
+    </row>
+    <row r="11" spans="2:57" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="131" t="s">
         <v>117</v>
       </c>
-      <c r="C10" s="26">
+      <c r="C11" s="26">
         <v>16</v>
       </c>
-      <c r="D10" s="26">
+      <c r="D11" s="26">
         <v>20</v>
       </c>
-      <c r="E10" s="26">
+      <c r="E11" s="26">
         <v>32</v>
       </c>
-      <c r="F10" s="26">
+      <c r="F11" s="26">
         <v>50</v>
       </c>
-      <c r="G10" s="26">
+      <c r="G11" s="26">
         <v>100</v>
       </c>
-      <c r="H10" s="26">
+      <c r="H11" s="26">
         <v>150</v>
       </c>
-      <c r="I10" s="26">
+      <c r="I11" s="26">
         <v>200</v>
       </c>
-      <c r="J10" s="26">
+      <c r="J11" s="26">
         <v>256</v>
       </c>
-      <c r="M10" s="131" t="s">
+      <c r="M11" s="131" t="s">
         <v>117</v>
       </c>
-      <c r="N10" s="26">
+      <c r="N11" s="26">
         <v>24</v>
       </c>
-      <c r="O10" s="26">
+      <c r="O11" s="26">
         <v>30</v>
       </c>
-      <c r="P10" s="26">
+      <c r="P11" s="26">
         <v>64</v>
       </c>
-      <c r="Q10" s="26">
+      <c r="Q11" s="26">
         <v>100</v>
       </c>
-      <c r="R10" s="26">
+      <c r="R11" s="26">
         <v>200</v>
       </c>
-      <c r="S10" s="26">
+      <c r="S11" s="26">
         <v>300</v>
       </c>
-      <c r="T10" s="26">
+      <c r="T11" s="26">
         <v>400</v>
       </c>
-      <c r="U10" s="26">
+      <c r="U11" s="26">
         <v>500</v>
       </c>
-      <c r="V10" s="26">
+      <c r="V11" s="26">
         <v>600</v>
       </c>
-      <c r="W10" s="26">
+      <c r="W11" s="26">
         <v>700</v>
       </c>
-      <c r="X10" s="26">
+      <c r="X11" s="26">
         <v>800</v>
       </c>
-      <c r="Y10" s="26">
+      <c r="Y11" s="26">
         <v>900</v>
       </c>
-      <c r="Z10" s="26">
+      <c r="Z11" s="26">
         <v>1000</v>
       </c>
-      <c r="AC10" s="131" t="s">
+      <c r="AC11" s="131" t="s">
         <v>117</v>
       </c>
-      <c r="AD10" s="26">
+      <c r="AD11" s="26">
         <v>20</v>
       </c>
-      <c r="AE10" s="26">
+      <c r="AE11" s="26">
         <v>25</v>
       </c>
-      <c r="AF10" s="26">
+      <c r="AF11" s="26">
         <v>40</v>
       </c>
-      <c r="AG10" s="26">
+      <c r="AG11" s="26">
         <v>50</v>
       </c>
-      <c r="AH10" s="26">
+      <c r="AH11" s="26">
         <v>100</v>
       </c>
-      <c r="AI10" s="26">
+      <c r="AI11" s="26">
         <v>200</v>
       </c>
-      <c r="AJ10" s="26">
+      <c r="AJ11" s="26">
         <v>300</v>
       </c>
-      <c r="AK10" s="26">
+      <c r="AK11" s="26">
         <v>397</v>
       </c>
-      <c r="AM10" s="95" t="s">
+      <c r="AM11" s="95" t="s">
         <v>117</v>
       </c>
-      <c r="AN10" s="26">
+      <c r="AN11" s="26">
         <v>5</v>
       </c>
-      <c r="AO10" s="26">
+      <c r="AO11" s="26">
         <v>10</v>
       </c>
-      <c r="AP10" s="26">
+      <c r="AP11" s="26">
         <v>20</v>
       </c>
-      <c r="AQ10" s="26">
+      <c r="AQ11" s="26">
         <v>30</v>
       </c>
-      <c r="AR10" s="26">
+      <c r="AR11" s="26">
         <v>40</v>
       </c>
-      <c r="AS10" s="26">
+      <c r="AS11" s="26">
         <v>50</v>
       </c>
-      <c r="AT10" s="26">
+      <c r="AT11" s="26">
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="2:57" x14ac:dyDescent="0.25">
-      <c r="B11" s="152" t="s">
+    <row r="12" spans="2:57" x14ac:dyDescent="0.25">
+      <c r="B12" s="152" t="s">
         <v>133</v>
       </c>
-      <c r="C11" s="58">
+      <c r="C12" s="58">
         <v>0.220786287579921</v>
       </c>
-      <c r="D11" s="58">
+      <c r="D12" s="58">
         <v>0.25302679907495601</v>
       </c>
-      <c r="E11" s="58">
+      <c r="E12" s="58">
         <v>0.32621412052781901</v>
       </c>
-      <c r="F11" s="58">
+      <c r="F12" s="58">
         <v>0.37858794721806599</v>
       </c>
-      <c r="G11" s="58">
+      <c r="G12" s="58">
         <v>0.43749149775540702</v>
       </c>
-      <c r="H11" s="58">
+      <c r="H12" s="58">
         <v>0.45993742347979899</v>
       </c>
-      <c r="I11" s="58">
+      <c r="I12" s="58">
         <v>0.47041218881784802</v>
       </c>
-      <c r="J11" s="58">
+      <c r="J12" s="58">
         <v>0.47816623588627399</v>
       </c>
-      <c r="M11" s="130" t="s">
+      <c r="K12" s="167"/>
+      <c r="M12" s="130" t="s">
         <v>133</v>
       </c>
-      <c r="N11" s="158">
+      <c r="N12" s="158">
         <v>8.4013333333333301E-2</v>
       </c>
-      <c r="O11" s="159">
+      <c r="O12" s="159">
         <v>0.10176</v>
       </c>
-      <c r="P11" s="159">
+      <c r="P12" s="159">
         <v>0.1457</v>
       </c>
-      <c r="Q11" s="159">
+      <c r="Q12" s="159">
         <v>0.16341333333333299</v>
       </c>
-      <c r="R11" s="159">
+      <c r="R12" s="159">
         <v>0.18308666666666701</v>
       </c>
-      <c r="S11" s="159">
+      <c r="S12" s="159">
         <v>0.19046666666666701</v>
       </c>
-      <c r="T11" s="159">
+      <c r="T12" s="159">
         <v>0.19536000000000001</v>
       </c>
-      <c r="U11" s="159">
+      <c r="U12" s="159">
         <v>0.198613333333333</v>
       </c>
-      <c r="V11" s="159">
+      <c r="V12" s="159">
         <v>0.20138</v>
       </c>
-      <c r="W11" s="159">
+      <c r="W12" s="159">
         <v>0.20376</v>
       </c>
-      <c r="X11" s="159">
+      <c r="X12" s="159">
         <v>0.20574666666666699</v>
       </c>
-      <c r="Y11" s="159">
+      <c r="Y12" s="159">
         <v>0.207386666666667</v>
       </c>
-      <c r="Z11" s="159">
+      <c r="Z12" s="159">
         <v>0.20854</v>
       </c>
-      <c r="AA11" s="167">
-        <f>AVERAGE(N11:Z11)</f>
+      <c r="AA12" s="167">
+        <f>AVERAGE(N12:Z12)</f>
         <v>0.17609435897435904</v>
       </c>
-      <c r="AC11" s="156" t="s">
+      <c r="AC12" s="156" t="s">
         <v>133</v>
       </c>
-      <c r="AD11" s="161">
+      <c r="AD12" s="161">
         <v>0.201597</v>
       </c>
-      <c r="AE11" s="161">
+      <c r="AE12" s="161">
         <v>0.23435900000000001</v>
       </c>
-      <c r="AF11" s="115">
+      <c r="AF12" s="115">
         <v>0.28938000000000003</v>
       </c>
-      <c r="AG11" s="159">
+      <c r="AG12" s="159">
         <v>0.31115959177636399</v>
       </c>
-      <c r="AH11" s="159">
+      <c r="AH12" s="159">
         <v>0.36407336192870898</v>
       </c>
-      <c r="AI11" s="159">
+      <c r="AI12" s="159">
         <v>0.40071734950451099</v>
       </c>
-      <c r="AJ11" s="159">
+      <c r="AJ12" s="159">
         <v>0.415803875166396</v>
       </c>
-      <c r="AK11" s="159">
+      <c r="AK12" s="159">
         <v>0.42312527732583899</v>
       </c>
-      <c r="AL11" s="167">
-        <f>AVERAGE(AD11:AK11)</f>
+      <c r="AL12" s="167">
+        <f>AVERAGE(AD12:AK12)</f>
         <v>0.33002693196272737</v>
       </c>
-      <c r="AM11" s="114" t="s">
+      <c r="AM12" s="114" t="s">
         <v>121</v>
       </c>
-      <c r="AN11" s="115">
+      <c r="AN12" s="115">
         <v>0.109239766081871</v>
       </c>
-      <c r="AO11" s="115">
+      <c r="AO12" s="115">
         <v>0.23485380116959101</v>
       </c>
-      <c r="AP11" s="115">
+      <c r="AP12" s="115">
         <v>0.29742690058479498</v>
       </c>
-      <c r="AQ11" s="115">
+      <c r="AQ12" s="115">
         <v>0.31684210526315798</v>
       </c>
-      <c r="AR11" s="115">
+      <c r="AR12" s="115">
         <v>0.32467836257309901</v>
       </c>
-      <c r="AS11" s="115">
+      <c r="AS12" s="115">
         <v>0.33099415204678401</v>
       </c>
-      <c r="AT11" s="115">
+      <c r="AT12" s="115">
         <v>0.336842105263158</v>
       </c>
     </row>
-    <row r="12" spans="2:57" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="153" t="s">
+    <row r="13" spans="2:57" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="153" t="s">
         <v>134</v>
-      </c>
-      <c r="C12" s="149">
-        <v>0.2283</v>
-      </c>
-      <c r="D12" s="149">
-        <v>0.26300000000000001</v>
-      </c>
-      <c r="E12" s="149">
-        <v>0.33529999999999999</v>
-      </c>
-      <c r="F12" s="149">
-        <v>0.38719999999999999</v>
-      </c>
-      <c r="G12" s="149">
-        <v>0.44779999999999998</v>
-      </c>
-      <c r="H12" s="149">
-        <v>0.47499999999999998</v>
-      </c>
-      <c r="I12" s="149">
-        <v>0.48770000000000002</v>
-      </c>
-      <c r="J12" s="122">
-        <v>0.4945</v>
-      </c>
-      <c r="M12" s="153" t="s">
-        <v>134</v>
-      </c>
-      <c r="N12" s="123">
-        <v>8.3299999999999999E-2</v>
-      </c>
-      <c r="O12" s="122">
-        <v>0.1008</v>
-      </c>
-      <c r="P12" s="122">
-        <v>0.14549999999999999</v>
-      </c>
-      <c r="Q12" s="122">
-        <v>0.16300000000000001</v>
-      </c>
-      <c r="R12" s="122">
-        <v>0.1825</v>
-      </c>
-      <c r="S12" s="122">
-        <v>0.18990000000000001</v>
-      </c>
-      <c r="T12" s="122">
-        <v>0.19439999999999999</v>
-      </c>
-      <c r="U12" s="122">
-        <v>0.19819999999999999</v>
-      </c>
-      <c r="V12" s="122">
-        <v>0.2006</v>
-      </c>
-      <c r="W12" s="122">
-        <v>0.2026</v>
-      </c>
-      <c r="X12" s="122">
-        <v>0.2041</v>
-      </c>
-      <c r="Y12" s="122">
-        <v>0.20619999999999999</v>
-      </c>
-      <c r="Z12" s="122">
-        <v>0.20730000000000001</v>
-      </c>
-      <c r="AA12" s="167">
-        <f t="shared" ref="AA12:AA17" si="0">AVERAGE(N12:Z12)</f>
-        <v>0.17526153846153841</v>
-      </c>
-      <c r="AC12" s="153" t="s">
-        <v>134</v>
-      </c>
-      <c r="AD12" s="150">
-        <v>0.2056</v>
-      </c>
-      <c r="AE12" s="150">
-        <v>0.24010000000000001</v>
-      </c>
-      <c r="AF12" s="149">
-        <v>0.29049999999999998</v>
-      </c>
-      <c r="AG12" s="120">
-        <v>0.30930000000000002</v>
-      </c>
-      <c r="AH12" s="120">
-        <v>0.35870000000000002</v>
-      </c>
-      <c r="AI12" s="120">
-        <v>0.39190000000000003</v>
-      </c>
-      <c r="AJ12" s="120">
-        <v>0.40699999999999997</v>
-      </c>
-      <c r="AK12" s="120">
-        <v>0.41649999999999998</v>
-      </c>
-      <c r="AL12" s="167">
-        <f t="shared" ref="AL12:AL22" si="1">AVERAGE(AD12:AK12)</f>
-        <v>0.32745000000000002</v>
-      </c>
-      <c r="AM12" s="29" t="s">
-        <v>120</v>
-      </c>
-      <c r="AN12" s="120"/>
-      <c r="AO12" s="120"/>
-      <c r="AP12" s="120"/>
-      <c r="AQ12" s="120"/>
-      <c r="AR12" s="120"/>
-      <c r="AS12" s="120"/>
-      <c r="AT12" s="120"/>
-    </row>
-    <row r="13" spans="2:57" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="29" t="s">
-        <v>137</v>
       </c>
       <c r="C13" s="149">
         <v>0.2283</v>
@@ -10620,8 +11153,8 @@
       <c r="J13" s="122">
         <v>0.4945</v>
       </c>
-      <c r="M13" s="29" t="s">
-        <v>137</v>
+      <c r="M13" s="153" t="s">
+        <v>134</v>
       </c>
       <c r="N13" s="123">
         <v>8.3299999999999999E-2</v>
@@ -10650,21 +11183,24 @@
       <c r="V13" s="122">
         <v>0.2006</v>
       </c>
-      <c r="W13" s="149">
+      <c r="W13" s="122">
         <v>0.2026</v>
       </c>
-      <c r="X13" s="149">
+      <c r="X13" s="122">
         <v>0.2041</v>
       </c>
-      <c r="Y13" s="149">
+      <c r="Y13" s="122">
         <v>0.20619999999999999</v>
       </c>
-      <c r="Z13" s="149">
+      <c r="Z13" s="122">
         <v>0.20730000000000001</v>
       </c>
-      <c r="AA13" s="167"/>
-      <c r="AC13" s="29" t="s">
-        <v>137</v>
+      <c r="AA13" s="167">
+        <f t="shared" ref="AA13:AA18" si="0">AVERAGE(N13:Z13)</f>
+        <v>0.17526153846153841</v>
+      </c>
+      <c r="AC13" s="153" t="s">
+        <v>134</v>
       </c>
       <c r="AD13" s="150">
         <v>0.2056</v>
@@ -10675,23 +11211,28 @@
       <c r="AF13" s="149">
         <v>0.29049999999999998</v>
       </c>
-      <c r="AG13" s="149">
+      <c r="AG13" s="120">
         <v>0.30930000000000002</v>
       </c>
-      <c r="AH13" s="149">
+      <c r="AH13" s="120">
         <v>0.35870000000000002</v>
       </c>
-      <c r="AI13" s="149">
+      <c r="AI13" s="120">
         <v>0.39190000000000003</v>
       </c>
-      <c r="AJ13" s="149">
+      <c r="AJ13" s="120">
         <v>0.40699999999999997</v>
       </c>
-      <c r="AK13" s="149">
+      <c r="AK13" s="120">
         <v>0.41649999999999998</v>
       </c>
-      <c r="AL13" s="167"/>
-      <c r="AM13" s="29"/>
+      <c r="AL13" s="167">
+        <f t="shared" ref="AL13:AL23" si="1">AVERAGE(AD13:AK13)</f>
+        <v>0.32745000000000002</v>
+      </c>
+      <c r="AM13" s="29" t="s">
+        <v>120</v>
+      </c>
       <c r="AN13" s="120"/>
       <c r="AO13" s="120"/>
       <c r="AP13" s="120"/>
@@ -10701,110 +11242,104 @@
       <c r="AT13" s="120"/>
     </row>
     <row r="14" spans="2:57" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C14" s="129">
-        <v>0.1583</v>
-      </c>
-      <c r="D14" s="129">
-        <v>0.18049999999999999</v>
-      </c>
-      <c r="E14" s="129">
-        <v>0.2419</v>
-      </c>
-      <c r="F14" s="129">
-        <v>0.29360000000000003</v>
-      </c>
-      <c r="G14" s="129">
-        <v>0.3745</v>
-      </c>
-      <c r="H14" s="129">
-        <v>0.4133</v>
-      </c>
-      <c r="I14" s="129">
-        <v>0.43419999999999997</v>
-      </c>
-      <c r="J14" s="129">
-        <v>0.4491</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="N14" s="160">
-        <v>8.8700000000000001E-2</v>
-      </c>
-      <c r="O14" s="160">
-        <v>0.1069</v>
-      </c>
-      <c r="P14" s="129">
-        <v>0.1525</v>
-      </c>
-      <c r="Q14" s="129">
-        <v>0.1696</v>
-      </c>
-      <c r="R14" s="160">
-        <v>0.18820000000000001</v>
-      </c>
-      <c r="S14" s="160">
-        <v>0.1953</v>
-      </c>
-      <c r="T14" s="160">
-        <v>0.19919999999999999</v>
-      </c>
-      <c r="U14" s="160">
-        <v>0.2011</v>
-      </c>
-      <c r="V14" s="160">
-        <v>0.20230000000000001</v>
-      </c>
-      <c r="W14" s="129">
-        <v>0.20300000000000001</v>
-      </c>
-      <c r="X14" s="129">
-        <v>0.20349999999999999</v>
-      </c>
-      <c r="Y14" s="129">
-        <v>0.20480000000000001</v>
-      </c>
-      <c r="Z14" s="129">
+      <c r="B14" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="C14" s="149">
+        <v>0.2283</v>
+      </c>
+      <c r="D14" s="149">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="E14" s="149">
+        <v>0.33529999999999999</v>
+      </c>
+      <c r="F14" s="149">
+        <v>0.38719999999999999</v>
+      </c>
+      <c r="G14" s="149">
+        <v>0.44779999999999998</v>
+      </c>
+      <c r="H14" s="149">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="I14" s="149">
+        <v>0.48770000000000002</v>
+      </c>
+      <c r="J14" s="122">
+        <v>0.4945</v>
+      </c>
+      <c r="M14" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="N14" s="123">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="O14" s="122">
+        <v>0.1008</v>
+      </c>
+      <c r="P14" s="122">
+        <v>0.14549999999999999</v>
+      </c>
+      <c r="Q14" s="122">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="R14" s="122">
+        <v>0.1825</v>
+      </c>
+      <c r="S14" s="122">
+        <v>0.18990000000000001</v>
+      </c>
+      <c r="T14" s="122">
+        <v>0.19439999999999999</v>
+      </c>
+      <c r="U14" s="122">
+        <v>0.19819999999999999</v>
+      </c>
+      <c r="V14" s="122">
+        <v>0.2006</v>
+      </c>
+      <c r="W14" s="149">
+        <v>0.2026</v>
+      </c>
+      <c r="X14" s="149">
+        <v>0.2041</v>
+      </c>
+      <c r="Y14" s="149">
+        <v>0.20619999999999999</v>
+      </c>
+      <c r="Z14" s="149">
+        <v>0.20730000000000001</v>
+      </c>
+      <c r="AA14" s="167"/>
+      <c r="AC14" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="AD14" s="150">
         <v>0.2056</v>
       </c>
-      <c r="AA14" s="167">
-        <f t="shared" si="0"/>
-        <v>0.1785153846153846</v>
-      </c>
-      <c r="AC14" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="AD14" s="162">
-        <v>7.9399999999999998E-2</v>
-      </c>
-      <c r="AE14" s="162">
-        <v>8.9899999999999994E-2</v>
-      </c>
-      <c r="AF14" s="162">
-        <v>0.10489999999999999</v>
-      </c>
-      <c r="AG14" s="162">
-        <v>0.1114</v>
-      </c>
-      <c r="AH14" s="162">
-        <v>0.13200000000000001</v>
-      </c>
-      <c r="AI14" s="162">
-        <v>0.14369999999999999</v>
-      </c>
-      <c r="AJ14" s="162">
-        <v>0.14580000000000001</v>
-      </c>
-      <c r="AK14" s="162">
-        <v>0.14680000000000001</v>
-      </c>
-      <c r="AL14" s="167">
-        <f t="shared" si="1"/>
-        <v>0.11923750000000001</v>
-      </c>
+      <c r="AE14" s="150">
+        <v>0.24010000000000001</v>
+      </c>
+      <c r="AF14" s="149">
+        <v>0.29049999999999998</v>
+      </c>
+      <c r="AG14" s="149">
+        <v>0.30930000000000002</v>
+      </c>
+      <c r="AH14" s="149">
+        <v>0.35870000000000002</v>
+      </c>
+      <c r="AI14" s="149">
+        <v>0.39190000000000003</v>
+      </c>
+      <c r="AJ14" s="149">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="AK14" s="149">
+        <v>0.41649999999999998</v>
+      </c>
+      <c r="AL14" s="167"/>
       <c r="AM14" s="29"/>
       <c r="AN14" s="120"/>
       <c r="AO14" s="120"/>
@@ -10815,109 +11350,109 @@
       <c r="AT14" s="120"/>
     </row>
     <row r="15" spans="2:57" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="71" t="s">
-        <v>139</v>
-      </c>
-      <c r="C15" s="74">
-        <v>0.13239999999999999</v>
-      </c>
-      <c r="D15" s="74">
-        <v>0.14080000000000001</v>
-      </c>
-      <c r="E15" s="74">
-        <v>0.16950000000000001</v>
-      </c>
-      <c r="F15" s="74">
-        <v>0.2072</v>
-      </c>
-      <c r="G15" s="74">
-        <v>0.24879999999999999</v>
-      </c>
-      <c r="H15" s="74">
-        <v>0.27710000000000001</v>
-      </c>
-      <c r="I15" s="74">
-        <v>0.3054</v>
-      </c>
-      <c r="J15" s="74">
-        <v>0.3538</v>
-      </c>
-      <c r="M15" s="71" t="s">
-        <v>139</v>
-      </c>
-      <c r="N15" s="74">
-        <v>4.3E-3</v>
-      </c>
-      <c r="O15" s="74">
-        <v>5.7000000000000002E-3</v>
-      </c>
-      <c r="P15" s="74">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="Q15" s="74">
-        <v>1.04E-2</v>
-      </c>
-      <c r="R15" s="74">
-        <v>1.8800000000000001E-2</v>
-      </c>
-      <c r="S15" s="74">
-        <v>2.58E-2</v>
-      </c>
-      <c r="T15" s="74">
-        <v>3.09E-2</v>
-      </c>
-      <c r="U15" s="74">
-        <v>3.4500000000000003E-2</v>
-      </c>
-      <c r="V15" s="74">
-        <v>3.8300000000000001E-2</v>
-      </c>
-      <c r="W15" s="74">
-        <v>4.2000000000000003E-2</v>
-      </c>
-      <c r="X15" s="74">
-        <v>4.4499999999999998E-2</v>
-      </c>
-      <c r="Y15" s="74">
-        <v>4.7899999999999998E-2</v>
-      </c>
-      <c r="Z15" s="74">
-        <v>5.0200000000000002E-2</v>
+      <c r="B15" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C15" s="129">
+        <v>0.1583</v>
+      </c>
+      <c r="D15" s="129">
+        <v>0.18049999999999999</v>
+      </c>
+      <c r="E15" s="129">
+        <v>0.2419</v>
+      </c>
+      <c r="F15" s="129">
+        <v>0.29360000000000003</v>
+      </c>
+      <c r="G15" s="129">
+        <v>0.3745</v>
+      </c>
+      <c r="H15" s="129">
+        <v>0.4133</v>
+      </c>
+      <c r="I15" s="129">
+        <v>0.43419999999999997</v>
+      </c>
+      <c r="J15" s="129">
+        <v>0.4491</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="N15" s="160">
+        <v>8.8700000000000001E-2</v>
+      </c>
+      <c r="O15" s="160">
+        <v>0.1069</v>
+      </c>
+      <c r="P15" s="129">
+        <v>0.1525</v>
+      </c>
+      <c r="Q15" s="129">
+        <v>0.1696</v>
+      </c>
+      <c r="R15" s="160">
+        <v>0.18820000000000001</v>
+      </c>
+      <c r="S15" s="160">
+        <v>0.1953</v>
+      </c>
+      <c r="T15" s="160">
+        <v>0.19919999999999999</v>
+      </c>
+      <c r="U15" s="160">
+        <v>0.2011</v>
+      </c>
+      <c r="V15" s="160">
+        <v>0.20230000000000001</v>
+      </c>
+      <c r="W15" s="129">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="X15" s="129">
+        <v>0.20349999999999999</v>
+      </c>
+      <c r="Y15" s="129">
+        <v>0.20480000000000001</v>
+      </c>
+      <c r="Z15" s="129">
+        <v>0.2056</v>
       </c>
       <c r="AA15" s="167">
         <f t="shared" si="0"/>
-        <v>2.7715384615384621E-2</v>
-      </c>
-      <c r="AC15" s="71" t="s">
-        <v>139</v>
-      </c>
-      <c r="AD15" s="163">
-        <v>7.9899999999999999E-2</v>
-      </c>
-      <c r="AE15" s="163">
-        <v>8.7099999999999997E-2</v>
-      </c>
-      <c r="AF15" s="163">
-        <v>0.1012</v>
-      </c>
-      <c r="AG15" s="163">
-        <v>0.1067</v>
-      </c>
-      <c r="AH15" s="163">
-        <v>0.1231</v>
-      </c>
-      <c r="AI15" s="163">
-        <v>0.13250000000000001</v>
-      </c>
-      <c r="AJ15" s="163">
-        <v>0.13370000000000001</v>
-      </c>
-      <c r="AK15" s="163">
-        <v>0.1343</v>
+        <v>0.1785153846153846</v>
+      </c>
+      <c r="AC15" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AD15" s="162">
+        <v>7.9399999999999998E-2</v>
+      </c>
+      <c r="AE15" s="162">
+        <v>8.9899999999999994E-2</v>
+      </c>
+      <c r="AF15" s="162">
+        <v>0.10489999999999999</v>
+      </c>
+      <c r="AG15" s="162">
+        <v>0.1114</v>
+      </c>
+      <c r="AH15" s="162">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="AI15" s="162">
+        <v>0.14369999999999999</v>
+      </c>
+      <c r="AJ15" s="162">
+        <v>0.14580000000000001</v>
+      </c>
+      <c r="AK15" s="162">
+        <v>0.14680000000000001</v>
       </c>
       <c r="AL15" s="167">
         <f t="shared" si="1"/>
-        <v>0.11231250000000001</v>
+        <v>0.11923750000000001</v>
       </c>
       <c r="AM15" s="29"/>
       <c r="AN15" s="120"/>
@@ -10928,110 +11463,110 @@
       <c r="AS15" s="120"/>
       <c r="AT15" s="120"/>
     </row>
-    <row r="16" spans="2:57" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="137" t="s">
-        <v>140</v>
-      </c>
-      <c r="C16" s="138">
-        <v>0.20349999999999999</v>
-      </c>
-      <c r="D16" s="138">
-        <v>0.23180000000000001</v>
-      </c>
-      <c r="E16" s="138">
-        <v>0.30959999999999999</v>
-      </c>
-      <c r="F16" s="138">
-        <v>0.36209999999999998</v>
-      </c>
-      <c r="G16" s="138">
-        <v>0.43690000000000001</v>
-      </c>
-      <c r="H16" s="138">
-        <v>0.47010000000000002</v>
-      </c>
-      <c r="I16" s="148">
-        <v>0.48770000000000002</v>
-      </c>
-      <c r="J16" s="148">
-        <v>0.50249999999999995</v>
-      </c>
-      <c r="M16" s="137" t="s">
-        <v>140</v>
-      </c>
-      <c r="N16" s="138">
-        <v>8.8300000000000003E-2</v>
-      </c>
-      <c r="O16" s="138">
-        <v>0.10680000000000001</v>
-      </c>
-      <c r="P16" s="148">
-        <v>0.15310000000000001</v>
-      </c>
-      <c r="Q16" s="148">
-        <v>0.16980000000000001</v>
-      </c>
-      <c r="R16" s="164">
-        <v>0.1862</v>
-      </c>
-      <c r="S16" s="138">
-        <v>0.19120000000000001</v>
-      </c>
-      <c r="T16" s="138">
-        <v>0.19159999999999999</v>
-      </c>
-      <c r="U16" s="138">
-        <v>0.19209999999999999</v>
-      </c>
-      <c r="V16" s="138">
-        <v>0.191</v>
-      </c>
-      <c r="W16" s="138">
-        <v>0.19020000000000001</v>
-      </c>
-      <c r="X16" s="138">
-        <v>0.1895</v>
-      </c>
-      <c r="Y16" s="138">
-        <v>0.1895</v>
-      </c>
-      <c r="Z16" s="138">
-        <v>0.1895</v>
+    <row r="16" spans="2:57" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="71" t="s">
+        <v>139</v>
+      </c>
+      <c r="C16" s="74">
+        <v>0.13239999999999999</v>
+      </c>
+      <c r="D16" s="74">
+        <v>0.14080000000000001</v>
+      </c>
+      <c r="E16" s="74">
+        <v>0.16950000000000001</v>
+      </c>
+      <c r="F16" s="74">
+        <v>0.2072</v>
+      </c>
+      <c r="G16" s="74">
+        <v>0.24879999999999999</v>
+      </c>
+      <c r="H16" s="74">
+        <v>0.27710000000000001</v>
+      </c>
+      <c r="I16" s="74">
+        <v>0.3054</v>
+      </c>
+      <c r="J16" s="74">
+        <v>0.3538</v>
+      </c>
+      <c r="M16" s="71" t="s">
+        <v>139</v>
+      </c>
+      <c r="N16" s="74">
+        <v>4.3E-3</v>
+      </c>
+      <c r="O16" s="74">
+        <v>5.7000000000000002E-3</v>
+      </c>
+      <c r="P16" s="74">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="Q16" s="74">
+        <v>1.04E-2</v>
+      </c>
+      <c r="R16" s="74">
+        <v>1.8800000000000001E-2</v>
+      </c>
+      <c r="S16" s="74">
+        <v>2.58E-2</v>
+      </c>
+      <c r="T16" s="74">
+        <v>3.09E-2</v>
+      </c>
+      <c r="U16" s="74">
+        <v>3.4500000000000003E-2</v>
+      </c>
+      <c r="V16" s="74">
+        <v>3.8300000000000001E-2</v>
+      </c>
+      <c r="W16" s="74">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="X16" s="74">
+        <v>4.4499999999999998E-2</v>
+      </c>
+      <c r="Y16" s="74">
+        <v>4.7899999999999998E-2</v>
+      </c>
+      <c r="Z16" s="74">
+        <v>5.0200000000000002E-2</v>
       </c>
       <c r="AA16" s="167">
         <f t="shared" si="0"/>
-        <v>0.17144615384615383</v>
-      </c>
-      <c r="AC16" s="137" t="s">
-        <v>140</v>
-      </c>
-      <c r="AD16" s="164">
-        <v>0.18629999999999999</v>
-      </c>
-      <c r="AE16" s="164">
-        <v>0.2094</v>
-      </c>
-      <c r="AF16" s="164">
-        <v>0.24709999999999999</v>
-      </c>
-      <c r="AG16" s="164">
-        <v>0.26240000000000002</v>
-      </c>
-      <c r="AH16" s="164">
-        <v>0.30570000000000003</v>
-      </c>
-      <c r="AI16" s="164">
-        <v>0.34339999999999998</v>
-      </c>
-      <c r="AJ16" s="164">
-        <v>0.36</v>
-      </c>
-      <c r="AK16" s="164">
-        <v>0.37119999999999997</v>
+        <v>2.7715384615384621E-2</v>
+      </c>
+      <c r="AC16" s="71" t="s">
+        <v>139</v>
+      </c>
+      <c r="AD16" s="163">
+        <v>7.9899999999999999E-2</v>
+      </c>
+      <c r="AE16" s="163">
+        <v>8.7099999999999997E-2</v>
+      </c>
+      <c r="AF16" s="163">
+        <v>0.1012</v>
+      </c>
+      <c r="AG16" s="163">
+        <v>0.1067</v>
+      </c>
+      <c r="AH16" s="163">
+        <v>0.1231</v>
+      </c>
+      <c r="AI16" s="163">
+        <v>0.13250000000000001</v>
+      </c>
+      <c r="AJ16" s="163">
+        <v>0.13370000000000001</v>
+      </c>
+      <c r="AK16" s="163">
+        <v>0.1343</v>
       </c>
       <c r="AL16" s="167">
         <f t="shared" si="1"/>
-        <v>0.28568749999999998</v>
+        <v>0.11231250000000001</v>
       </c>
       <c r="AM16" s="29"/>
       <c r="AN16" s="120"/>
@@ -11042,110 +11577,110 @@
       <c r="AS16" s="120"/>
       <c r="AT16" s="120"/>
     </row>
-    <row r="17" spans="2:46" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="154" t="s">
-        <v>135</v>
-      </c>
-      <c r="C17" s="84">
-        <v>0.22159999999999999</v>
-      </c>
-      <c r="D17" s="84">
-        <v>0.25359999999999999</v>
-      </c>
-      <c r="E17" s="84">
-        <v>0.32529999999999998</v>
-      </c>
-      <c r="F17" s="127">
-        <v>0.36919999999999997</v>
-      </c>
-      <c r="G17" s="127">
-        <v>0.41499999999999998</v>
-      </c>
-      <c r="H17" s="127">
-        <v>0.42480000000000001</v>
-      </c>
-      <c r="I17" s="127">
-        <v>0.42759999999999998</v>
-      </c>
-      <c r="J17" s="127">
-        <v>0.42880000000000001</v>
-      </c>
-      <c r="M17" s="154" t="s">
-        <v>135</v>
-      </c>
-      <c r="N17" s="127">
-        <v>8.0799999999999997E-2</v>
-      </c>
-      <c r="O17" s="127">
-        <v>9.7600000000000006E-2</v>
-      </c>
-      <c r="P17" s="127">
-        <v>0.1391</v>
-      </c>
-      <c r="Q17" s="127">
-        <v>0.15409999999999999</v>
-      </c>
-      <c r="R17" s="127">
-        <v>0.17180000000000001</v>
-      </c>
-      <c r="S17" s="127">
-        <v>0.17799999999999999</v>
-      </c>
-      <c r="T17" s="127">
-        <v>0.18090000000000001</v>
-      </c>
-      <c r="U17" s="127">
-        <v>0.18360000000000001</v>
-      </c>
-      <c r="V17" s="127">
-        <v>0.185</v>
-      </c>
-      <c r="W17" s="127">
-        <v>0.185</v>
-      </c>
-      <c r="X17" s="127">
-        <v>0.18579999999999999</v>
-      </c>
-      <c r="Y17" s="127">
-        <v>0.18590000000000001</v>
-      </c>
-      <c r="Z17" s="127">
-        <v>0.18579999999999999</v>
+    <row r="17" spans="2:46" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="137" t="s">
+        <v>140</v>
+      </c>
+      <c r="C17" s="138">
+        <v>0.20349999999999999</v>
+      </c>
+      <c r="D17" s="138">
+        <v>0.23180000000000001</v>
+      </c>
+      <c r="E17" s="138">
+        <v>0.30959999999999999</v>
+      </c>
+      <c r="F17" s="138">
+        <v>0.36209999999999998</v>
+      </c>
+      <c r="G17" s="138">
+        <v>0.43690000000000001</v>
+      </c>
+      <c r="H17" s="138">
+        <v>0.47010000000000002</v>
+      </c>
+      <c r="I17" s="148">
+        <v>0.48770000000000002</v>
+      </c>
+      <c r="J17" s="148">
+        <v>0.50249999999999995</v>
+      </c>
+      <c r="M17" s="137" t="s">
+        <v>140</v>
+      </c>
+      <c r="N17" s="138">
+        <v>8.8300000000000003E-2</v>
+      </c>
+      <c r="O17" s="138">
+        <v>0.10680000000000001</v>
+      </c>
+      <c r="P17" s="148">
+        <v>0.15310000000000001</v>
+      </c>
+      <c r="Q17" s="148">
+        <v>0.16980000000000001</v>
+      </c>
+      <c r="R17" s="164">
+        <v>0.1862</v>
+      </c>
+      <c r="S17" s="138">
+        <v>0.19120000000000001</v>
+      </c>
+      <c r="T17" s="138">
+        <v>0.19159999999999999</v>
+      </c>
+      <c r="U17" s="138">
+        <v>0.19209999999999999</v>
+      </c>
+      <c r="V17" s="138">
+        <v>0.191</v>
+      </c>
+      <c r="W17" s="138">
+        <v>0.19020000000000001</v>
+      </c>
+      <c r="X17" s="138">
+        <v>0.1895</v>
+      </c>
+      <c r="Y17" s="138">
+        <v>0.1895</v>
+      </c>
+      <c r="Z17" s="138">
+        <v>0.1895</v>
       </c>
       <c r="AA17" s="167">
         <f t="shared" si="0"/>
-        <v>0.16256923076923077</v>
-      </c>
-      <c r="AC17" s="154" t="s">
-        <v>135</v>
-      </c>
-      <c r="AD17" s="84">
-        <v>0.2026</v>
-      </c>
-      <c r="AE17" s="84">
-        <v>0.2336</v>
-      </c>
-      <c r="AF17" s="84">
-        <v>0.28920000000000001</v>
-      </c>
-      <c r="AG17" s="84">
-        <v>0.30959999999999999</v>
-      </c>
-      <c r="AH17" s="84">
-        <v>0.35599999999999998</v>
-      </c>
-      <c r="AI17" s="84">
-        <v>0.3735</v>
-      </c>
-      <c r="AJ17" s="84">
-        <v>0.37830000000000003</v>
-      </c>
-      <c r="AK17" s="84">
-        <v>0.37819999999999998</v>
+        <v>0.17144615384615383</v>
+      </c>
+      <c r="AC17" s="137" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD17" s="164">
+        <v>0.18629999999999999</v>
+      </c>
+      <c r="AE17" s="164">
+        <v>0.2094</v>
+      </c>
+      <c r="AF17" s="164">
+        <v>0.24709999999999999</v>
+      </c>
+      <c r="AG17" s="164">
+        <v>0.26240000000000002</v>
+      </c>
+      <c r="AH17" s="164">
+        <v>0.30570000000000003</v>
+      </c>
+      <c r="AI17" s="164">
+        <v>0.34339999999999998</v>
+      </c>
+      <c r="AJ17" s="164">
+        <v>0.36</v>
+      </c>
+      <c r="AK17" s="164">
+        <v>0.37119999999999997</v>
       </c>
       <c r="AL17" s="167">
         <f t="shared" si="1"/>
-        <v>0.31512499999999999</v>
+        <v>0.28568749999999998</v>
       </c>
       <c r="AM17" s="29"/>
       <c r="AN17" s="120"/>
@@ -11156,17 +11691,17 @@
       <c r="AS17" s="120"/>
       <c r="AT17" s="120"/>
     </row>
-    <row r="18" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B18" s="73" t="s">
-        <v>141</v>
-      </c>
-      <c r="C18" s="82">
+    <row r="18" spans="2:46" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="154" t="s">
+        <v>135</v>
+      </c>
+      <c r="C18" s="84">
         <v>0.22159999999999999</v>
       </c>
-      <c r="D18" s="82">
+      <c r="D18" s="84">
         <v>0.25359999999999999</v>
       </c>
-      <c r="E18" s="82">
+      <c r="E18" s="84">
         <v>0.32529999999999998</v>
       </c>
       <c r="F18" s="127">
@@ -11184,8 +11719,8 @@
       <c r="J18" s="127">
         <v>0.42880000000000001</v>
       </c>
-      <c r="M18" s="73" t="s">
-        <v>141</v>
+      <c r="M18" s="154" t="s">
+        <v>135</v>
       </c>
       <c r="N18" s="127">
         <v>8.0799999999999997E-2</v>
@@ -11226,35 +11761,41 @@
       <c r="Z18" s="127">
         <v>0.18579999999999999</v>
       </c>
-      <c r="AA18" s="167"/>
-      <c r="AC18" s="73" t="s">
-        <v>141</v>
-      </c>
-      <c r="AD18" s="82">
+      <c r="AA18" s="167">
+        <f t="shared" si="0"/>
+        <v>0.16256923076923077</v>
+      </c>
+      <c r="AC18" s="154" t="s">
+        <v>135</v>
+      </c>
+      <c r="AD18" s="84">
         <v>0.2026</v>
       </c>
-      <c r="AE18" s="82">
+      <c r="AE18" s="84">
         <v>0.2336</v>
       </c>
-      <c r="AF18" s="82">
+      <c r="AF18" s="84">
         <v>0.28920000000000001</v>
       </c>
-      <c r="AG18" s="82">
+      <c r="AG18" s="84">
         <v>0.30959999999999999</v>
       </c>
-      <c r="AH18" s="82">
+      <c r="AH18" s="84">
         <v>0.35599999999999998</v>
       </c>
-      <c r="AI18" s="82">
+      <c r="AI18" s="84">
         <v>0.3735</v>
       </c>
-      <c r="AJ18" s="82">
+      <c r="AJ18" s="84">
         <v>0.37830000000000003</v>
       </c>
-      <c r="AK18" s="82">
+      <c r="AK18" s="84">
         <v>0.37819999999999998</v>
       </c>
-      <c r="AL18" s="167"/>
+      <c r="AL18" s="167">
+        <f t="shared" si="1"/>
+        <v>0.31512499999999999</v>
+      </c>
       <c r="AM18" s="29"/>
       <c r="AN18" s="120"/>
       <c r="AO18" s="120"/>
@@ -11264,107 +11805,105 @@
       <c r="AS18" s="120"/>
       <c r="AT18" s="120"/>
     </row>
-    <row r="19" spans="2:46" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="62" t="s">
-        <v>142</v>
-      </c>
-      <c r="C19" s="94">
-        <v>0.16919999999999999</v>
-      </c>
-      <c r="D19" s="94">
-        <v>0.18870000000000001</v>
-      </c>
-      <c r="E19" s="94">
-        <v>0.24679999999999999</v>
-      </c>
-      <c r="F19" s="94">
-        <v>0.3</v>
-      </c>
-      <c r="G19" s="94">
-        <v>0.35399999999999998</v>
-      </c>
-      <c r="H19" s="94">
-        <v>0.3715</v>
-      </c>
-      <c r="I19" s="94">
-        <v>0.37869999999999998</v>
-      </c>
-      <c r="J19" s="94">
-        <v>0.38429999999999997</v>
-      </c>
-      <c r="M19" s="62" t="s">
-        <v>142</v>
-      </c>
-      <c r="N19" s="121">
-        <v>8.5400000000000004E-2</v>
-      </c>
-      <c r="O19" s="121">
-        <v>0.1028</v>
-      </c>
-      <c r="P19" s="121">
-        <v>0.1459</v>
-      </c>
-      <c r="Q19" s="121">
-        <v>0.16139999999999999</v>
-      </c>
-      <c r="R19" s="121">
-        <v>0.1797</v>
-      </c>
-      <c r="S19" s="121">
-        <v>0.18609999999999999</v>
-      </c>
-      <c r="T19" s="121">
-        <v>0.1893</v>
-      </c>
-      <c r="U19" s="121">
-        <v>0.1918</v>
-      </c>
-      <c r="V19" s="121">
-        <v>0.1928</v>
-      </c>
-      <c r="W19" s="121">
-        <v>0.19309999999999999</v>
-      </c>
-      <c r="X19" s="121">
-        <v>0.19350000000000001</v>
-      </c>
-      <c r="Y19" s="121">
-        <v>0.19359999999999999</v>
-      </c>
-      <c r="Z19" s="121">
-        <v>0.19339999999999999</v>
-      </c>
-      <c r="AC19" s="62" t="s">
-        <v>142</v>
-      </c>
-      <c r="AD19" s="121">
-        <v>0.1358</v>
-      </c>
-      <c r="AE19" s="121">
-        <v>0.15079999999999999</v>
-      </c>
-      <c r="AF19" s="121">
-        <v>0.18529999999999999</v>
-      </c>
-      <c r="AG19" s="121">
-        <v>0.20050000000000001</v>
-      </c>
-      <c r="AH19" s="121">
-        <v>0.2379</v>
-      </c>
-      <c r="AI19" s="121">
-        <v>0.25580000000000003</v>
-      </c>
-      <c r="AJ19" s="121">
-        <v>0.25900000000000001</v>
-      </c>
-      <c r="AK19" s="121">
-        <v>0.25900000000000001</v>
-      </c>
-      <c r="AL19" s="167">
-        <f t="shared" si="1"/>
-        <v>0.21051249999999999</v>
-      </c>
+    <row r="19" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="B19" s="73" t="s">
+        <v>141</v>
+      </c>
+      <c r="C19" s="82">
+        <v>0.22159999999999999</v>
+      </c>
+      <c r="D19" s="82">
+        <v>0.25359999999999999</v>
+      </c>
+      <c r="E19" s="82">
+        <v>0.32529999999999998</v>
+      </c>
+      <c r="F19" s="127">
+        <v>0.36919999999999997</v>
+      </c>
+      <c r="G19" s="127">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="H19" s="127">
+        <v>0.42480000000000001</v>
+      </c>
+      <c r="I19" s="127">
+        <v>0.42759999999999998</v>
+      </c>
+      <c r="J19" s="127">
+        <v>0.42880000000000001</v>
+      </c>
+      <c r="M19" s="73" t="s">
+        <v>141</v>
+      </c>
+      <c r="N19" s="127">
+        <v>8.0799999999999997E-2</v>
+      </c>
+      <c r="O19" s="127">
+        <v>9.7600000000000006E-2</v>
+      </c>
+      <c r="P19" s="127">
+        <v>0.1391</v>
+      </c>
+      <c r="Q19" s="127">
+        <v>0.15409999999999999</v>
+      </c>
+      <c r="R19" s="127">
+        <v>0.17180000000000001</v>
+      </c>
+      <c r="S19" s="127">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="T19" s="127">
+        <v>0.18090000000000001</v>
+      </c>
+      <c r="U19" s="127">
+        <v>0.18360000000000001</v>
+      </c>
+      <c r="V19" s="127">
+        <v>0.185</v>
+      </c>
+      <c r="W19" s="127">
+        <v>0.185</v>
+      </c>
+      <c r="X19" s="127">
+        <v>0.18579999999999999</v>
+      </c>
+      <c r="Y19" s="127">
+        <v>0.18590000000000001</v>
+      </c>
+      <c r="Z19" s="127">
+        <v>0.18579999999999999</v>
+      </c>
+      <c r="AA19" s="167"/>
+      <c r="AC19" s="73" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD19" s="82">
+        <v>0.2026</v>
+      </c>
+      <c r="AE19" s="82">
+        <v>0.2336</v>
+      </c>
+      <c r="AF19" s="82">
+        <v>0.28920000000000001</v>
+      </c>
+      <c r="AG19" s="82">
+        <v>0.30959999999999999</v>
+      </c>
+      <c r="AH19" s="82">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="AI19" s="82">
+        <v>0.3735</v>
+      </c>
+      <c r="AJ19" s="82">
+        <v>0.37830000000000003</v>
+      </c>
+      <c r="AK19" s="82">
+        <v>0.37819999999999998</v>
+      </c>
+      <c r="AL19" s="167"/>
       <c r="AM19" s="29"/>
       <c r="AN19" s="120"/>
       <c r="AO19" s="120"/>
@@ -11375,105 +11914,105 @@
       <c r="AT19" s="120"/>
     </row>
     <row r="20" spans="2:46" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="132" t="s">
-        <v>143</v>
-      </c>
-      <c r="C20" s="133">
-        <v>0.13250000000000001</v>
-      </c>
-      <c r="D20" s="133">
-        <v>0.14580000000000001</v>
-      </c>
-      <c r="E20" s="133">
-        <v>0.17829999999999999</v>
-      </c>
-      <c r="F20" s="133">
-        <v>0.21179999999999999</v>
-      </c>
-      <c r="G20" s="133">
-        <v>0.2601</v>
-      </c>
-      <c r="H20" s="133">
-        <v>0.2742</v>
-      </c>
-      <c r="I20" s="133">
-        <v>0.27860000000000001</v>
-      </c>
-      <c r="J20" s="133">
-        <v>0.27900000000000003</v>
-      </c>
-      <c r="M20" s="132" t="s">
-        <v>143</v>
-      </c>
-      <c r="N20" s="133">
-        <v>3.9600000000000003E-2</v>
-      </c>
-      <c r="O20" s="133">
-        <v>4.4200000000000003E-2</v>
-      </c>
-      <c r="P20" s="133">
-        <v>6.9199999999999998E-2</v>
-      </c>
-      <c r="Q20" s="133">
-        <v>8.3299999999999999E-2</v>
-      </c>
-      <c r="R20" s="133">
-        <v>0.10150000000000001</v>
-      </c>
-      <c r="S20" s="133">
-        <v>0.1109</v>
-      </c>
-      <c r="T20" s="133">
-        <v>0.1159</v>
-      </c>
-      <c r="U20" s="133">
-        <v>0.11899999999999999</v>
-      </c>
-      <c r="V20" s="133">
-        <v>0.1205</v>
-      </c>
-      <c r="W20" s="133">
-        <v>0.12180000000000001</v>
-      </c>
-      <c r="X20" s="133">
-        <v>0.1217</v>
-      </c>
-      <c r="Y20" s="133">
-        <v>0.122</v>
-      </c>
-      <c r="Z20" s="133">
-        <v>0.12189999999999999</v>
-      </c>
-      <c r="AC20" s="132" t="s">
-        <v>143</v>
-      </c>
-      <c r="AD20" s="133">
-        <v>0.1421</v>
-      </c>
-      <c r="AE20" s="133">
-        <v>0.15459999999999999</v>
-      </c>
-      <c r="AF20" s="133">
-        <v>0.18459999999999999</v>
-      </c>
-      <c r="AG20" s="133">
-        <v>0.1963</v>
-      </c>
-      <c r="AH20" s="133">
-        <v>0.22220000000000001</v>
-      </c>
-      <c r="AI20" s="133">
-        <v>0.2293</v>
-      </c>
-      <c r="AJ20" s="133">
-        <v>0.23050000000000001</v>
-      </c>
-      <c r="AK20" s="133">
-        <v>0.23069999999999999</v>
+      <c r="B20" s="62" t="s">
+        <v>142</v>
+      </c>
+      <c r="C20" s="94">
+        <v>0.16919999999999999</v>
+      </c>
+      <c r="D20" s="94">
+        <v>0.18870000000000001</v>
+      </c>
+      <c r="E20" s="94">
+        <v>0.24679999999999999</v>
+      </c>
+      <c r="F20" s="94">
+        <v>0.3</v>
+      </c>
+      <c r="G20" s="94">
+        <v>0.35399999999999998</v>
+      </c>
+      <c r="H20" s="94">
+        <v>0.3715</v>
+      </c>
+      <c r="I20" s="94">
+        <v>0.37869999999999998</v>
+      </c>
+      <c r="J20" s="94">
+        <v>0.38429999999999997</v>
+      </c>
+      <c r="M20" s="62" t="s">
+        <v>142</v>
+      </c>
+      <c r="N20" s="121">
+        <v>8.5400000000000004E-2</v>
+      </c>
+      <c r="O20" s="121">
+        <v>0.1028</v>
+      </c>
+      <c r="P20" s="121">
+        <v>0.1459</v>
+      </c>
+      <c r="Q20" s="121">
+        <v>0.16139999999999999</v>
+      </c>
+      <c r="R20" s="121">
+        <v>0.1797</v>
+      </c>
+      <c r="S20" s="121">
+        <v>0.18609999999999999</v>
+      </c>
+      <c r="T20" s="121">
+        <v>0.1893</v>
+      </c>
+      <c r="U20" s="121">
+        <v>0.1918</v>
+      </c>
+      <c r="V20" s="121">
+        <v>0.1928</v>
+      </c>
+      <c r="W20" s="121">
+        <v>0.19309999999999999</v>
+      </c>
+      <c r="X20" s="121">
+        <v>0.19350000000000001</v>
+      </c>
+      <c r="Y20" s="121">
+        <v>0.19359999999999999</v>
+      </c>
+      <c r="Z20" s="121">
+        <v>0.19339999999999999</v>
+      </c>
+      <c r="AC20" s="62" t="s">
+        <v>142</v>
+      </c>
+      <c r="AD20" s="121">
+        <v>0.1358</v>
+      </c>
+      <c r="AE20" s="121">
+        <v>0.15079999999999999</v>
+      </c>
+      <c r="AF20" s="121">
+        <v>0.18529999999999999</v>
+      </c>
+      <c r="AG20" s="121">
+        <v>0.20050000000000001</v>
+      </c>
+      <c r="AH20" s="121">
+        <v>0.2379</v>
+      </c>
+      <c r="AI20" s="121">
+        <v>0.25580000000000003</v>
+      </c>
+      <c r="AJ20" s="121">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="AK20" s="121">
+        <v>0.25900000000000001</v>
       </c>
       <c r="AL20" s="167">
         <f t="shared" si="1"/>
-        <v>0.19878749999999998</v>
+        <v>0.21051249999999999</v>
       </c>
       <c r="AM20" s="29"/>
       <c r="AN20" s="120"/>
@@ -11484,110 +12023,108 @@
       <c r="AS20" s="120"/>
       <c r="AT20" s="120"/>
     </row>
-    <row r="21" spans="2:46" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="137" t="s">
-        <v>144</v>
-      </c>
-      <c r="C21" s="139">
-        <v>0.217</v>
-      </c>
-      <c r="D21" s="139">
-        <v>0.248</v>
-      </c>
-      <c r="E21" s="139">
-        <v>0.31469999999999998</v>
-      </c>
-      <c r="F21" s="147">
-        <v>0.37180000000000002</v>
-      </c>
-      <c r="G21" s="147">
-        <v>0.42330000000000001</v>
-      </c>
-      <c r="H21" s="147">
-        <v>0.4365</v>
-      </c>
-      <c r="I21" s="147">
-        <v>0.43790000000000001</v>
-      </c>
-      <c r="J21" s="147">
-        <v>0.43709999999999999</v>
-      </c>
-      <c r="M21" s="137" t="s">
-        <v>144</v>
-      </c>
-      <c r="N21" s="147">
-        <v>8.6800000000000002E-2</v>
-      </c>
-      <c r="O21" s="147">
-        <v>0.10489999999999999</v>
-      </c>
-      <c r="P21" s="147">
-        <v>0.1507</v>
-      </c>
-      <c r="Q21" s="147">
-        <v>0.16639999999999999</v>
-      </c>
-      <c r="R21" s="147">
-        <v>0.1847</v>
-      </c>
-      <c r="S21" s="147">
-        <v>0.19209999999999999</v>
-      </c>
-      <c r="T21" s="147">
-        <v>0.1953</v>
-      </c>
-      <c r="U21" s="147">
-        <v>0.19739999999999999</v>
-      </c>
-      <c r="V21" s="147">
-        <v>0.19889999999999999</v>
-      </c>
-      <c r="W21" s="147">
-        <v>0.19950000000000001</v>
-      </c>
-      <c r="X21" s="147">
-        <v>0.19939999999999999</v>
-      </c>
-      <c r="Y21" s="147">
-        <v>0.19950000000000001</v>
-      </c>
-      <c r="Z21" s="147">
-        <v>0.19939999999999999</v>
-      </c>
-      <c r="AC21" s="137" t="s">
-        <v>144</v>
-      </c>
-      <c r="AD21" s="139">
-        <v>0.19270000000000001</v>
-      </c>
-      <c r="AE21" s="139">
-        <v>0.22289999999999999</v>
-      </c>
-      <c r="AF21" s="139">
-        <v>0.27550000000000002</v>
-      </c>
-      <c r="AG21" s="139">
-        <v>0.29670000000000002</v>
-      </c>
-      <c r="AH21" s="139">
-        <v>0.34499999999999997</v>
-      </c>
-      <c r="AI21" s="139">
-        <v>0.36549999999999999</v>
-      </c>
-      <c r="AJ21" s="139">
-        <v>0.37030000000000002</v>
-      </c>
-      <c r="AK21" s="139">
-        <v>0.3705</v>
+    <row r="21" spans="2:46" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="132" t="s">
+        <v>143</v>
+      </c>
+      <c r="C21" s="133">
+        <v>0.13250000000000001</v>
+      </c>
+      <c r="D21" s="133">
+        <v>0.14580000000000001</v>
+      </c>
+      <c r="E21" s="133">
+        <v>0.17829999999999999</v>
+      </c>
+      <c r="F21" s="133">
+        <v>0.21179999999999999</v>
+      </c>
+      <c r="G21" s="133">
+        <v>0.2601</v>
+      </c>
+      <c r="H21" s="133">
+        <v>0.2742</v>
+      </c>
+      <c r="I21" s="133">
+        <v>0.27860000000000001</v>
+      </c>
+      <c r="J21" s="133">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="M21" s="132" t="s">
+        <v>143</v>
+      </c>
+      <c r="N21" s="133">
+        <v>3.9600000000000003E-2</v>
+      </c>
+      <c r="O21" s="133">
+        <v>4.4200000000000003E-2</v>
+      </c>
+      <c r="P21" s="133">
+        <v>6.9199999999999998E-2</v>
+      </c>
+      <c r="Q21" s="133">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="R21" s="133">
+        <v>0.10150000000000001</v>
+      </c>
+      <c r="S21" s="133">
+        <v>0.1109</v>
+      </c>
+      <c r="T21" s="133">
+        <v>0.1159</v>
+      </c>
+      <c r="U21" s="133">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="V21" s="133">
+        <v>0.1205</v>
+      </c>
+      <c r="W21" s="133">
+        <v>0.12180000000000001</v>
+      </c>
+      <c r="X21" s="133">
+        <v>0.1217</v>
+      </c>
+      <c r="Y21" s="133">
+        <v>0.122</v>
+      </c>
+      <c r="Z21" s="133">
+        <v>0.12189999999999999</v>
+      </c>
+      <c r="AC21" s="132" t="s">
+        <v>143</v>
+      </c>
+      <c r="AD21" s="133">
+        <v>0.1421</v>
+      </c>
+      <c r="AE21" s="133">
+        <v>0.15459999999999999</v>
+      </c>
+      <c r="AF21" s="133">
+        <v>0.18459999999999999</v>
+      </c>
+      <c r="AG21" s="133">
+        <v>0.1963</v>
+      </c>
+      <c r="AH21" s="133">
+        <v>0.22220000000000001</v>
+      </c>
+      <c r="AI21" s="133">
+        <v>0.2293</v>
+      </c>
+      <c r="AJ21" s="133">
+        <v>0.23050000000000001</v>
+      </c>
+      <c r="AK21" s="133">
+        <v>0.23069999999999999</v>
       </c>
       <c r="AL21" s="167">
         <f t="shared" si="1"/>
-        <v>0.30488749999999998</v>
-      </c>
-      <c r="AM21" s="29" t="s">
-        <v>120</v>
-      </c>
+        <v>0.19878749999999998</v>
+      </c>
+      <c r="AM21" s="29"/>
       <c r="AN21" s="120"/>
       <c r="AO21" s="120"/>
       <c r="AP21" s="120"/>
@@ -11596,277 +12133,389 @@
       <c r="AS21" s="120"/>
       <c r="AT21" s="120"/>
     </row>
-    <row r="22" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B22" s="155" t="s">
-        <v>136</v>
-      </c>
-      <c r="C22" s="128">
-        <v>4.2599999999999999E-2</v>
-      </c>
-      <c r="D22" s="128">
-        <v>4.9399999999999999E-2</v>
-      </c>
-      <c r="E22" s="128">
-        <v>5.4300000000000001E-2</v>
-      </c>
-      <c r="F22" s="128">
-        <v>6.7900000000000002E-2</v>
-      </c>
-      <c r="G22" s="128">
-        <v>0.1341</v>
-      </c>
-      <c r="H22" s="128">
-        <v>0.24809999999999999</v>
-      </c>
-      <c r="I22" s="128">
-        <v>0.37669999999999998</v>
-      </c>
-      <c r="J22" s="151">
-        <v>0.50170000000000003</v>
-      </c>
-      <c r="M22" s="134" t="s">
-        <v>136</v>
-      </c>
-      <c r="N22" s="135">
-        <v>1.2500000000000001E-2</v>
-      </c>
-      <c r="O22" s="128">
-        <v>1.46E-2</v>
-      </c>
-      <c r="P22" s="128">
-        <v>2.2599999999999999E-2</v>
-      </c>
-      <c r="Q22" s="128">
-        <v>3.0599999999999999E-2</v>
-      </c>
-      <c r="R22" s="128">
-        <v>4.99E-2</v>
-      </c>
-      <c r="S22" s="128">
-        <v>7.0400000000000004E-2</v>
-      </c>
-      <c r="T22" s="128">
-        <v>8.9399999999999993E-2</v>
-      </c>
-      <c r="U22" s="128">
-        <v>0.1079</v>
-      </c>
-      <c r="V22" s="128">
-        <v>0.12870000000000001</v>
-      </c>
-      <c r="W22" s="128">
-        <v>0.14729999999999999</v>
-      </c>
-      <c r="X22" s="128">
-        <v>0.1656</v>
-      </c>
-      <c r="Y22" s="128">
-        <v>0.1837</v>
-      </c>
-      <c r="Z22" s="128">
-        <v>0.20619999999999999</v>
-      </c>
-      <c r="AC22" s="157" t="s">
-        <v>136</v>
-      </c>
-      <c r="AD22" s="165">
-        <v>8.8599999999999998E-2</v>
-      </c>
-      <c r="AE22" s="165">
-        <v>0.1096</v>
-      </c>
-      <c r="AF22" s="166">
-        <v>0.14449999999999999</v>
-      </c>
-      <c r="AG22" s="166">
-        <v>0.1177</v>
-      </c>
-      <c r="AH22" s="166">
-        <v>0.26329999999999998</v>
-      </c>
-      <c r="AI22" s="166">
-        <v>0.3543</v>
-      </c>
-      <c r="AJ22" s="166">
-        <v>0.39360000000000001</v>
-      </c>
-      <c r="AK22" s="166">
-        <v>0.43330000000000002</v>
+    <row r="22" spans="2:46" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="137" t="s">
+        <v>144</v>
+      </c>
+      <c r="C22" s="139">
+        <v>0.217</v>
+      </c>
+      <c r="D22" s="139">
+        <v>0.248</v>
+      </c>
+      <c r="E22" s="139">
+        <v>0.31469999999999998</v>
+      </c>
+      <c r="F22" s="147">
+        <v>0.37180000000000002</v>
+      </c>
+      <c r="G22" s="147">
+        <v>0.42330000000000001</v>
+      </c>
+      <c r="H22" s="147">
+        <v>0.4365</v>
+      </c>
+      <c r="I22" s="147">
+        <v>0.43790000000000001</v>
+      </c>
+      <c r="J22" s="147">
+        <v>0.43709999999999999</v>
+      </c>
+      <c r="M22" s="137" t="s">
+        <v>144</v>
+      </c>
+      <c r="N22" s="147">
+        <v>8.6800000000000002E-2</v>
+      </c>
+      <c r="O22" s="147">
+        <v>0.10489999999999999</v>
+      </c>
+      <c r="P22" s="147">
+        <v>0.1507</v>
+      </c>
+      <c r="Q22" s="147">
+        <v>0.16639999999999999</v>
+      </c>
+      <c r="R22" s="147">
+        <v>0.1847</v>
+      </c>
+      <c r="S22" s="147">
+        <v>0.19209999999999999</v>
+      </c>
+      <c r="T22" s="147">
+        <v>0.1953</v>
+      </c>
+      <c r="U22" s="147">
+        <v>0.19739999999999999</v>
+      </c>
+      <c r="V22" s="147">
+        <v>0.19889999999999999</v>
+      </c>
+      <c r="W22" s="147">
+        <v>0.19950000000000001</v>
+      </c>
+      <c r="X22" s="147">
+        <v>0.19939999999999999</v>
+      </c>
+      <c r="Y22" s="147">
+        <v>0.19950000000000001</v>
+      </c>
+      <c r="Z22" s="147">
+        <v>0.19939999999999999</v>
+      </c>
+      <c r="AC22" s="137" t="s">
+        <v>144</v>
+      </c>
+      <c r="AD22" s="139">
+        <v>0.19270000000000001</v>
+      </c>
+      <c r="AE22" s="139">
+        <v>0.22289999999999999</v>
+      </c>
+      <c r="AF22" s="139">
+        <v>0.27550000000000002</v>
+      </c>
+      <c r="AG22" s="139">
+        <v>0.29670000000000002</v>
+      </c>
+      <c r="AH22" s="139">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="AI22" s="139">
+        <v>0.36549999999999999</v>
+      </c>
+      <c r="AJ22" s="139">
+        <v>0.37030000000000002</v>
+      </c>
+      <c r="AK22" s="139">
+        <v>0.3705</v>
       </c>
       <c r="AL22" s="167">
         <f t="shared" si="1"/>
+        <v>0.30488749999999998</v>
+      </c>
+      <c r="AM22" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="AN22" s="120"/>
+      <c r="AO22" s="120"/>
+      <c r="AP22" s="120"/>
+      <c r="AQ22" s="120"/>
+      <c r="AR22" s="120"/>
+      <c r="AS22" s="120"/>
+      <c r="AT22" s="120"/>
+    </row>
+    <row r="23" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="B23" s="155" t="s">
+        <v>136</v>
+      </c>
+      <c r="C23" s="128">
+        <v>4.2599999999999999E-2</v>
+      </c>
+      <c r="D23" s="128">
+        <v>4.9399999999999999E-2</v>
+      </c>
+      <c r="E23" s="128">
+        <v>5.4300000000000001E-2</v>
+      </c>
+      <c r="F23" s="128">
+        <v>6.7900000000000002E-2</v>
+      </c>
+      <c r="G23" s="128">
+        <v>0.1341</v>
+      </c>
+      <c r="H23" s="128">
+        <v>0.24809999999999999</v>
+      </c>
+      <c r="I23" s="128">
+        <v>0.37669999999999998</v>
+      </c>
+      <c r="J23" s="151">
+        <v>0.50170000000000003</v>
+      </c>
+      <c r="M23" s="134" t="s">
+        <v>136</v>
+      </c>
+      <c r="N23" s="135">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="O23" s="128">
+        <v>1.46E-2</v>
+      </c>
+      <c r="P23" s="128">
+        <v>2.2599999999999999E-2</v>
+      </c>
+      <c r="Q23" s="128">
+        <v>3.0599999999999999E-2</v>
+      </c>
+      <c r="R23" s="128">
+        <v>4.99E-2</v>
+      </c>
+      <c r="S23" s="128">
+        <v>7.0400000000000004E-2</v>
+      </c>
+      <c r="T23" s="128">
+        <v>8.9399999999999993E-2</v>
+      </c>
+      <c r="U23" s="128">
+        <v>0.1079</v>
+      </c>
+      <c r="V23" s="128">
+        <v>0.12870000000000001</v>
+      </c>
+      <c r="W23" s="128">
+        <v>0.14729999999999999</v>
+      </c>
+      <c r="X23" s="128">
+        <v>0.1656</v>
+      </c>
+      <c r="Y23" s="128">
+        <v>0.1837</v>
+      </c>
+      <c r="Z23" s="128">
+        <v>0.20619999999999999</v>
+      </c>
+      <c r="AC23" s="157" t="s">
+        <v>136</v>
+      </c>
+      <c r="AD23" s="165">
+        <v>8.8599999999999998E-2</v>
+      </c>
+      <c r="AE23" s="165">
+        <v>0.1096</v>
+      </c>
+      <c r="AF23" s="166">
+        <v>0.14449999999999999</v>
+      </c>
+      <c r="AG23" s="166">
+        <v>0.1177</v>
+      </c>
+      <c r="AH23" s="166">
+        <v>0.26329999999999998</v>
+      </c>
+      <c r="AI23" s="166">
+        <v>0.3543</v>
+      </c>
+      <c r="AJ23" s="166">
+        <v>0.39360000000000001</v>
+      </c>
+      <c r="AK23" s="166">
+        <v>0.43330000000000002</v>
+      </c>
+      <c r="AL23" s="167">
+        <f t="shared" si="1"/>
         <v>0.2381125</v>
       </c>
-      <c r="AM22" s="62" t="s">
+      <c r="AM23" s="62" t="s">
         <v>116</v>
       </c>
-      <c r="AN22" s="121">
+      <c r="AN23" s="121">
         <v>1.7500000000000002E-2</v>
       </c>
-      <c r="AO22" s="121">
+      <c r="AO23" s="121">
         <v>1.7500000000000002E-2</v>
       </c>
-      <c r="AP22" s="121">
+      <c r="AP23" s="121">
         <v>1.7899999999999999E-2</v>
       </c>
-      <c r="AQ22" s="121">
+      <c r="AQ23" s="121">
         <v>2.6200000000000001E-2</v>
       </c>
-      <c r="AR22" s="121">
+      <c r="AR23" s="121">
         <v>5.1299999999999998E-2</v>
       </c>
-      <c r="AS22" s="121">
+      <c r="AS23" s="121">
         <v>8.3500000000000005E-2</v>
       </c>
-      <c r="AT22" s="121">
+      <c r="AT23" s="121">
         <v>0.38479999999999998</v>
       </c>
     </row>
-    <row r="23" spans="2:46" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="136" t="s">
+    <row r="24" spans="2:46" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="136" t="s">
         <v>119</v>
       </c>
-      <c r="C23" s="118">
+      <c r="C24" s="118">
         <v>0.24579999999999999</v>
       </c>
-      <c r="D23" s="118">
+      <c r="D24" s="118">
         <v>0.28649999999999998</v>
       </c>
-      <c r="E23" s="118">
+      <c r="E24" s="118">
         <v>0.35709999999999997</v>
       </c>
-      <c r="F23" s="118">
+      <c r="F24" s="118">
         <v>0.40060000000000001</v>
       </c>
-      <c r="G23" s="118">
+      <c r="G24" s="118">
         <v>0.46079999999999999</v>
       </c>
-      <c r="H23" s="118">
+      <c r="H24" s="118">
         <v>0.48180000000000001</v>
       </c>
-      <c r="I23" s="118">
+      <c r="I24" s="118">
         <v>0.49149999999999999</v>
       </c>
-      <c r="J23" s="118">
+      <c r="J24" s="118">
         <v>0.50170000000000003</v>
       </c>
-      <c r="M23" s="136" t="s">
+      <c r="M24" s="136" t="s">
         <v>119</v>
       </c>
-      <c r="N23" s="117">
+      <c r="N24" s="117">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="O23" s="118">
+      <c r="O24" s="118">
         <v>0.1056</v>
       </c>
-      <c r="P23" s="118">
+      <c r="P24" s="118">
         <v>0.1472</v>
       </c>
-      <c r="Q23" s="118">
+      <c r="Q24" s="118">
         <v>0.16300000000000001</v>
       </c>
-      <c r="R23" s="118">
+      <c r="R24" s="118">
         <v>0.18390000000000001</v>
       </c>
-      <c r="S23" s="118">
+      <c r="S24" s="118">
         <v>0.1908</v>
       </c>
-      <c r="T23" s="118">
+      <c r="T24" s="118">
         <v>0.19670000000000001</v>
       </c>
-      <c r="U23" s="118">
+      <c r="U24" s="118">
         <v>0.1991</v>
       </c>
-      <c r="V23" s="118">
+      <c r="V24" s="118">
         <v>0.20150000000000001</v>
       </c>
-      <c r="W23" s="118">
+      <c r="W24" s="118">
         <v>0.2031</v>
       </c>
-      <c r="X23" s="118">
+      <c r="X24" s="118">
         <v>0.2039</v>
       </c>
-      <c r="Y23" s="118">
+      <c r="Y24" s="118">
         <v>0.20480000000000001</v>
       </c>
-      <c r="Z23" s="118">
+      <c r="Z24" s="118">
         <v>0.20619999999999999</v>
       </c>
-      <c r="AA23" s="167">
-        <f>AA12-AA17</f>
+      <c r="AA24" s="167">
+        <f>AA13-AA18</f>
         <v>1.2692307692307642E-2</v>
       </c>
-      <c r="AC23" s="136" t="s">
+      <c r="AC24" s="136" t="s">
         <v>119</v>
       </c>
-      <c r="AD23" s="117">
+      <c r="AD24" s="117">
         <v>0.23669999999999999</v>
       </c>
-      <c r="AE23" s="117">
+      <c r="AE24" s="117">
         <v>0.26860000000000001</v>
       </c>
-      <c r="AF23" s="118">
+      <c r="AF24" s="118">
         <v>0.32329999999999998</v>
       </c>
-      <c r="AG23" s="118">
+      <c r="AG24" s="118">
         <v>0.34250000000000003</v>
       </c>
-      <c r="AH23" s="118">
+      <c r="AH24" s="118">
         <v>0.38429999999999997</v>
       </c>
-      <c r="AI23" s="118">
+      <c r="AI24" s="118">
         <v>0.4138</v>
       </c>
-      <c r="AJ23" s="118">
+      <c r="AJ24" s="118">
         <v>0.42699999999999999</v>
       </c>
-      <c r="AK23" s="118">
+      <c r="AK24" s="118">
         <v>0.43330000000000002</v>
       </c>
-      <c r="AM23" s="116" t="s">
+      <c r="AM24" s="116" t="s">
         <v>119</v>
       </c>
-      <c r="AN23" s="119">
+      <c r="AN24" s="119">
         <v>0.13189999999999999</v>
       </c>
-      <c r="AO23" s="119">
+      <c r="AO24" s="119">
         <v>0.2581</v>
       </c>
-      <c r="AP23" s="119">
+      <c r="AP24" s="119">
         <v>0.33250000000000002</v>
       </c>
-      <c r="AQ23" s="119">
+      <c r="AQ24" s="119">
         <v>0.35630000000000001</v>
       </c>
-      <c r="AR23" s="119">
+      <c r="AR24" s="119">
         <v>0.37269999999999998</v>
       </c>
-      <c r="AS23" s="119">
+      <c r="AS24" s="119">
         <v>0.38200000000000001</v>
       </c>
-      <c r="AT23" s="119">
+      <c r="AT24" s="119">
         <v>0.38479999999999998</v>
       </c>
     </row>
-    <row r="24" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="AA24" s="167">
-        <f>AA11-AA12</f>
+    <row r="25" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="AA25" s="167">
+        <f>AA12-AA13</f>
         <v>8.3282051282063119E-4</v>
       </c>
-      <c r="AL24" s="167">
-        <f>AL11-AL12</f>
+      <c r="AL25" s="167">
+        <f>AL12-AL13</f>
         <v>2.5769319627273468E-3</v>
       </c>
     </row>
-    <row r="25" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="AL25" s="167">
-        <f>AL12-AL17</f>
+    <row r="26" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="AL26" s="167">
+        <f>AL13-AL18</f>
         <v>1.232500000000003E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="C7:J7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -12228,8 +12877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q46"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12419,4 +13068,210 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E23"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="97" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="59.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C2" s="180">
+        <v>0.20619999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B4" s="168" t="s">
+        <v>188</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="124"/>
+      <c r="B5" s="168" t="s">
+        <v>240</v>
+      </c>
+      <c r="C5" s="62" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="126"/>
+      <c r="B6" s="179"/>
+      <c r="C6" s="170"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>32</v>
+      </c>
+      <c r="B7" s="175" t="s">
+        <v>228</v>
+      </c>
+      <c r="C7" s="172"/>
+      <c r="D7" s="172"/>
+      <c r="E7" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="176" t="s">
+        <v>229</v>
+      </c>
+      <c r="C8" s="172"/>
+      <c r="D8" s="172"/>
+      <c r="E8" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="175" t="s">
+        <v>230</v>
+      </c>
+      <c r="C9" s="172"/>
+      <c r="D9" s="172"/>
+      <c r="E9" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="176" t="s">
+        <v>231</v>
+      </c>
+      <c r="C10" s="172"/>
+      <c r="D10" s="172"/>
+      <c r="E10" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="177" t="s">
+        <v>232</v>
+      </c>
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="178" t="s">
+        <v>233</v>
+      </c>
+      <c r="C12" s="73"/>
+      <c r="D12" s="73"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="177" t="s">
+        <v>234</v>
+      </c>
+      <c r="C13" s="73"/>
+      <c r="D13" s="73"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="178" t="s">
+        <v>235</v>
+      </c>
+      <c r="C14" s="73"/>
+      <c r="D14" s="73"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>210</v>
+      </c>
+      <c r="B16" s="171" t="s">
+        <v>206</v>
+      </c>
+      <c r="C16" s="172"/>
+      <c r="D16" s="172"/>
+      <c r="E16" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="172" t="s">
+        <v>203</v>
+      </c>
+      <c r="C17" s="172"/>
+      <c r="D17" s="172"/>
+      <c r="E17" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="171" t="s">
+        <v>207</v>
+      </c>
+      <c r="C18" s="172"/>
+      <c r="D18" s="172"/>
+      <c r="E18" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="172" t="s">
+        <v>202</v>
+      </c>
+      <c r="C19" s="172"/>
+      <c r="D19" s="172"/>
+      <c r="E19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="169" t="s">
+        <v>208</v>
+      </c>
+      <c r="C20" s="73"/>
+      <c r="D20" s="73"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="173" t="s">
+        <v>204</v>
+      </c>
+      <c r="C21" s="73"/>
+      <c r="D21" s="73"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="169" t="s">
+        <v>209</v>
+      </c>
+      <c r="C22" s="73"/>
+      <c r="D22" s="73"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="173" t="s">
+        <v>205</v>
+      </c>
+      <c r="C23" s="173"/>
+      <c r="D23" s="73"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>